<commit_message>
them test case 1
</commit_message>
<xml_diff>
--- a/Project_Code_Testcase_Template_v2.2.xlsx
+++ b/Project_Code_Testcase_Template_v2.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\OneDrive - Hanoi University of Science and Technology\BaiGiang\Quantriduan\DemoTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nam4-1\Quan Tri Du An\QuanTriDuAnCNTT-CNTT-20181\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{C2329458-F936-4E58-B5C2-98927AEFA968}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{DA92033F-E7E2-40F0-97C5-4B82ECF31751}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1D0CE496-6F6F-4E48-A396-5C94805316ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$51</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -30,21 +30,7 @@
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Point \ Point 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="H27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="J27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="H29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="I29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -111,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="J29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="A30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -156,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="H31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="I31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -200,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
   <si>
     <t>Online ID</t>
   </si>
@@ -211,37 +197,19 @@
     <t>23/08/2008</t>
   </si>
   <si>
-    <t>BUG21312</t>
-  </si>
-  <si>
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
-    <t>Test với tham số mặc định</t>
-  </si>
-  <si>
     <t>1.1-1</t>
   </si>
   <si>
     <t>1.1-2</t>
   </si>
   <si>
-    <t>Test với tham số chỉ định</t>
-  </si>
-  <si>
-    <t>2.1.</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
     <t>2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test với tham số chỉ định \ Test với tham số -r </t>
-  </si>
-  <si>
-    <t>1.2.1-1</t>
   </si>
   <si>
     <t>1.2.2-2</t>
@@ -355,19 +323,6 @@
 3. Gõ địa chỉ 192.168.0.5</t>
   </si>
   <si>
-    <t xml:space="preserve">Không có tham số dòng lệnh
-</t>
-  </si>
-  <si>
-    <t>1. Gõ duy nhất tên chương trình, không có tham số dòng lệnh</t>
-  </si>
-  <si>
-    <t>Chạy được</t>
-  </si>
-  <si>
-    <t>Không có tham số dòng lệnh, nhưng nhập từ Task Manager</t>
-  </si>
-  <si>
     <t>File Mpeg có thời lượng 3s</t>
   </si>
   <si>
@@ -423,6 +378,48 @@
   </si>
   <si>
     <t>Hear and Note</t>
+  </si>
+  <si>
+    <t>Test đăng nhập</t>
+  </si>
+  <si>
+    <t>Không nhập tài khoản hoặc mật khẩu</t>
+  </si>
+  <si>
+    <t>chỉ nhập tên tài khoản hoặc mật khẩu, hoặc không nhập cả tài khoản và mật khẩu</t>
+  </si>
+  <si>
+    <t>hiển thị thông báo yêu cầu nhập tài khoản, mật khẩu</t>
+  </si>
+  <si>
+    <t>DungVV</t>
+  </si>
+  <si>
+    <t>14/12/2018</t>
+  </si>
+  <si>
+    <t>Nhập sai mật khẩu</t>
+  </si>
+  <si>
+    <t>nhập mật khẩu sai</t>
+  </si>
+  <si>
+    <t>hiển thị thông báo nhập mật khẩu sai, yêu cầu nhập lại mật khẩu</t>
+  </si>
+  <si>
+    <t>1.1-3</t>
+  </si>
+  <si>
+    <t>nhập đúng tài khoản và mật khẩu</t>
+  </si>
+  <si>
+    <t>nhập tài khoản và mật khẩu đã được tạo</t>
+  </si>
+  <si>
+    <t>đăng nhập thành công</t>
+  </si>
+  <si>
+    <t>Test chức năng</t>
   </si>
 </sst>
 </file>
@@ -613,7 +610,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,6 +668,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="24"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,7 +936,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1021,12 +1024,6 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1036,9 +1033,6 @@
     <xf numFmtId="1" fontId="21" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1065,15 +1059,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1184,9 +1169,6 @@
     <xf numFmtId="49" fontId="20" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1238,94 +1220,139 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1755,8 +1782,8 @@
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1795,13 +1822,13 @@
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
-      <c r="V2" s="79"/>
+      <c r="V2" s="73"/>
       <c r="W2" s="13"/>
       <c r="X2" s="14"/>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1815,7 +1842,7 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
-      <c r="N3" s="78"/>
+      <c r="N3" s="72"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
@@ -1823,7 +1850,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
-      <c r="V3" s="80"/>
+      <c r="V3" s="74"/>
       <c r="W3" s="18"/>
       <c r="X3" s="19"/>
     </row>
@@ -1882,13 +1909,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="127" t="s">
-        <v>15</v>
-      </c>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
+      <c r="O6" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="120"/>
+      <c r="Q6" s="120"/>
+      <c r="R6" s="120"/>
+      <c r="S6" s="120"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1898,11 +1925,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="Q7" s="127"/>
-      <c r="R7" s="127"/>
-      <c r="S7" s="127"/>
+      <c r="O7" s="120"/>
+      <c r="P7" s="120"/>
+      <c r="Q7" s="120"/>
+      <c r="R7" s="120"/>
+      <c r="S7" s="120"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -1911,37 +1938,37 @@
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="31"/>
-      <c r="X8" s="77"/>
+      <c r="X8" s="71"/>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1">
       <c r="B9" s="30"/>
       <c r="C9" s="18"/>
       <c r="D9" s="27" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="82"/>
+      <c r="H9" s="76"/>
       <c r="X9" s="19"/>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1">
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="27" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="82"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
-      <c r="L10" s="124" t="s">
-        <v>24</v>
+      <c r="L10" s="117" t="s">
+        <v>18</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
@@ -1955,34 +1982,34 @@
       <c r="B11" s="30"/>
       <c r="C11" s="18"/>
       <c r="D11" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="128">
+        <v>11</v>
+      </c>
+      <c r="E11" s="121">
         <f ca="1">TODAY()</f>
-        <v>43206</v>
-      </c>
-      <c r="F11" s="128"/>
-      <c r="G11" s="128"/>
-      <c r="H11" s="82"/>
+        <v>43448</v>
+      </c>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="76"/>
       <c r="L11" s="33" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="V11" s="33"/>
       <c r="X11" s="19"/>
@@ -1990,27 +2017,27 @@
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
       <c r="L12" s="34" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="73">
+      <c r="O12" s="67">
         <v>2</v>
       </c>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="74">
+      <c r="P12" s="67"/>
+      <c r="Q12" s="68">
         <v>3</v>
       </c>
-      <c r="R12" s="74"/>
-      <c r="S12" s="75">
+      <c r="R12" s="68"/>
+      <c r="S12" s="69">
         <v>4</v>
       </c>
-      <c r="T12" s="75"/>
-      <c r="U12" s="76">
+      <c r="T12" s="69"/>
+      <c r="U12" s="70">
         <f t="shared" ref="U12:U18" si="0">SUM(O12:T12)</f>
         <v>9</v>
       </c>
-      <c r="V12" s="76"/>
+      <c r="V12" s="70"/>
       <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:24">
@@ -2020,23 +2047,23 @@
       </c>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
-      <c r="O13" s="73">
+      <c r="O13" s="67">
         <v>22</v>
       </c>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="74">
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68">
         <v>22</v>
       </c>
-      <c r="R13" s="74"/>
-      <c r="S13" s="75">
+      <c r="R13" s="68"/>
+      <c r="S13" s="69">
         <v>22</v>
       </c>
-      <c r="T13" s="75"/>
-      <c r="U13" s="76">
+      <c r="T13" s="69"/>
+      <c r="U13" s="70">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="V13" s="76"/>
+      <c r="V13" s="70"/>
       <c r="X13" s="19"/>
     </row>
     <row r="14" spans="1:24">
@@ -2046,56 +2073,56 @@
       </c>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="73">
+      <c r="O14" s="67">
         <v>32</v>
       </c>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="74">
+      <c r="P14" s="67"/>
+      <c r="Q14" s="68">
         <v>32</v>
       </c>
-      <c r="R14" s="74"/>
-      <c r="S14" s="75">
+      <c r="R14" s="68"/>
+      <c r="S14" s="69">
         <v>32</v>
       </c>
-      <c r="T14" s="75"/>
-      <c r="U14" s="76">
+      <c r="T14" s="69"/>
+      <c r="U14" s="70">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="V14" s="76"/>
+      <c r="V14" s="70"/>
       <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
+        <v>39</v>
+      </c>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
       <c r="L15" s="34">
         <v>4</v>
       </c>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
-      <c r="O15" s="73">
+      <c r="O15" s="67">
         <v>42</v>
       </c>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="74">
+      <c r="P15" s="67"/>
+      <c r="Q15" s="68">
         <v>42</v>
       </c>
-      <c r="R15" s="74"/>
-      <c r="S15" s="75">
+      <c r="R15" s="68"/>
+      <c r="S15" s="69">
         <v>42</v>
       </c>
-      <c r="T15" s="75"/>
-      <c r="U15" s="76">
+      <c r="T15" s="69"/>
+      <c r="U15" s="70">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="V15" s="76"/>
+      <c r="V15" s="70"/>
       <c r="X15" s="19"/>
     </row>
     <row r="16" spans="1:24">
@@ -2110,23 +2137,23 @@
       </c>
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
-      <c r="O16" s="73">
+      <c r="O16" s="67">
         <v>52</v>
       </c>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="74">
+      <c r="P16" s="67"/>
+      <c r="Q16" s="68">
         <v>52</v>
       </c>
-      <c r="R16" s="74"/>
-      <c r="S16" s="75">
+      <c r="R16" s="68"/>
+      <c r="S16" s="69">
         <v>52</v>
       </c>
-      <c r="T16" s="75"/>
-      <c r="U16" s="76">
+      <c r="T16" s="69"/>
+      <c r="U16" s="70">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="V16" s="76"/>
+      <c r="V16" s="70"/>
       <c r="X16" s="19"/>
     </row>
     <row r="17" spans="2:35">
@@ -2141,23 +2168,23 @@
       </c>
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
-      <c r="O17" s="73">
+      <c r="O17" s="67">
         <v>62</v>
       </c>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="74">
+      <c r="P17" s="67"/>
+      <c r="Q17" s="68">
         <v>62</v>
       </c>
-      <c r="R17" s="74"/>
-      <c r="S17" s="75">
+      <c r="R17" s="68"/>
+      <c r="S17" s="69">
         <v>62</v>
       </c>
-      <c r="T17" s="75"/>
-      <c r="U17" s="76">
+      <c r="T17" s="69"/>
+      <c r="U17" s="70">
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="V17" s="76"/>
+      <c r="V17" s="70"/>
       <c r="X17" s="19"/>
     </row>
     <row r="18" spans="2:35">
@@ -2172,23 +2199,23 @@
       </c>
       <c r="M18" s="35"/>
       <c r="N18" s="35"/>
-      <c r="O18" s="73">
+      <c r="O18" s="67">
         <v>72</v>
       </c>
-      <c r="P18" s="73"/>
-      <c r="Q18" s="74">
+      <c r="P18" s="67"/>
+      <c r="Q18" s="68">
         <v>72</v>
       </c>
-      <c r="R18" s="74"/>
-      <c r="S18" s="75">
+      <c r="R18" s="68"/>
+      <c r="S18" s="69">
         <v>72</v>
       </c>
-      <c r="T18" s="75"/>
-      <c r="U18" s="76">
+      <c r="T18" s="69"/>
+      <c r="U18" s="70">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="V18" s="76"/>
+      <c r="V18" s="70"/>
       <c r="X18" s="19"/>
     </row>
     <row r="19" spans="2:35">
@@ -2199,31 +2226,31 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="L19" s="36" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
-      <c r="O19" s="122">
+      <c r="O19" s="115">
         <f>SUM(O12:O18)</f>
         <v>284</v>
       </c>
-      <c r="P19" s="122"/>
-      <c r="Q19" s="122">
+      <c r="P19" s="115"/>
+      <c r="Q19" s="115">
         <f>SUM(Q12:Q18)</f>
         <v>285</v>
       </c>
-      <c r="R19" s="122"/>
-      <c r="S19" s="122">
+      <c r="R19" s="115"/>
+      <c r="S19" s="115">
         <f>SUM(S12:S18)</f>
         <v>286</v>
       </c>
-      <c r="T19" s="122"/>
-      <c r="U19" s="123">
+      <c r="T19" s="115"/>
+      <c r="U19" s="116">
         <f>SUM(U12:U18)</f>
         <v>855</v>
       </c>
-      <c r="V19" s="123"/>
-      <c r="W19" s="84"/>
+      <c r="V19" s="116"/>
+      <c r="W19" s="78"/>
       <c r="X19" s="19"/>
     </row>
     <row r="20" spans="2:35">
@@ -2251,12 +2278,12 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
+        <v>40</v>
+      </c>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
       <c r="W22" s="17"/>
       <c r="X22" s="23"/>
     </row>
@@ -2267,7 +2294,7 @@
       <c r="F23" s="44"/>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
-      <c r="W23" s="85"/>
+      <c r="W23" s="79"/>
       <c r="X23" s="23"/>
     </row>
     <row r="24" spans="2:35" s="17" customFormat="1">
@@ -2277,20 +2304,20 @@
       <c r="F24" s="44"/>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
-      <c r="L24" s="124" t="s">
-        <v>67</v>
-      </c>
-      <c r="M24" s="114"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="114"/>
-      <c r="P24" s="115"/>
-      <c r="Q24" s="115"/>
-      <c r="R24" s="115"/>
-      <c r="S24" s="115"/>
-      <c r="T24" s="115"/>
-      <c r="U24" s="115"/>
-      <c r="V24" s="115"/>
-      <c r="W24" s="83"/>
+      <c r="L24" s="117" t="s">
+        <v>57</v>
+      </c>
+      <c r="M24" s="107"/>
+      <c r="N24" s="107"/>
+      <c r="O24" s="107"/>
+      <c r="P24" s="108"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="108"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="108"/>
+      <c r="U24" s="108"/>
+      <c r="V24" s="108"/>
+      <c r="W24" s="77"/>
       <c r="X24" s="23"/>
     </row>
     <row r="25" spans="2:35" s="17" customFormat="1">
@@ -2299,18 +2326,18 @@
       <c r="F25" s="44"/>
       <c r="G25" s="44"/>
       <c r="H25" s="44"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="117"/>
-      <c r="N25" s="117"/>
-      <c r="O25" s="117"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="118"/>
-      <c r="S25" s="118"/>
-      <c r="T25" s="118"/>
-      <c r="U25" s="118"/>
-      <c r="V25" s="118"/>
-      <c r="W25" s="83"/>
+      <c r="L25" s="109"/>
+      <c r="M25" s="110"/>
+      <c r="N25" s="110"/>
+      <c r="O25" s="110"/>
+      <c r="P25" s="111"/>
+      <c r="Q25" s="111"/>
+      <c r="R25" s="111"/>
+      <c r="S25" s="111"/>
+      <c r="T25" s="111"/>
+      <c r="U25" s="111"/>
+      <c r="V25" s="111"/>
+      <c r="W25" s="77"/>
       <c r="X25" s="23"/>
     </row>
     <row r="26" spans="2:35" s="17" customFormat="1">
@@ -2319,58 +2346,58 @@
       <c r="F26" s="44"/>
       <c r="G26" s="44"/>
       <c r="H26" s="44"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="117"/>
-      <c r="N26" s="117"/>
-      <c r="O26" s="117"/>
-      <c r="P26" s="118"/>
-      <c r="Q26" s="118"/>
-      <c r="R26" s="118"/>
-      <c r="S26" s="118"/>
-      <c r="T26" s="118"/>
-      <c r="U26" s="118"/>
-      <c r="V26" s="118"/>
-      <c r="W26" s="83"/>
+      <c r="L26" s="109"/>
+      <c r="M26" s="110"/>
+      <c r="N26" s="110"/>
+      <c r="O26" s="110"/>
+      <c r="P26" s="111"/>
+      <c r="Q26" s="111"/>
+      <c r="R26" s="111"/>
+      <c r="S26" s="111"/>
+      <c r="T26" s="111"/>
+      <c r="U26" s="111"/>
+      <c r="V26" s="111"/>
+      <c r="W26" s="77"/>
       <c r="X26" s="23"/>
-      <c r="AB26" s="86"/>
+      <c r="AB26" s="80"/>
     </row>
     <row r="27" spans="2:35" s="17" customFormat="1">
       <c r="B27" s="22"/>
       <c r="D27" s="38"/>
       <c r="E27" s="4"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="117"/>
-      <c r="N27" s="117"/>
-      <c r="O27" s="117"/>
-      <c r="P27" s="118"/>
-      <c r="Q27" s="118"/>
-      <c r="R27" s="118"/>
-      <c r="S27" s="118"/>
-      <c r="T27" s="118"/>
-      <c r="U27" s="118"/>
-      <c r="V27" s="118"/>
-      <c r="W27" s="83"/>
+      <c r="L27" s="109"/>
+      <c r="M27" s="110"/>
+      <c r="N27" s="110"/>
+      <c r="O27" s="110"/>
+      <c r="P27" s="111"/>
+      <c r="Q27" s="111"/>
+      <c r="R27" s="111"/>
+      <c r="S27" s="111"/>
+      <c r="T27" s="111"/>
+      <c r="U27" s="111"/>
+      <c r="V27" s="111"/>
+      <c r="W27" s="77"/>
       <c r="X27" s="23"/>
-      <c r="AB27" s="86"/>
+      <c r="AB27" s="80"/>
     </row>
     <row r="28" spans="2:35" s="17" customFormat="1">
       <c r="B28" s="22"/>
       <c r="D28" s="38"/>
       <c r="E28" s="4"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="117"/>
-      <c r="N28" s="117"/>
-      <c r="O28" s="117"/>
-      <c r="P28" s="118"/>
-      <c r="Q28" s="118"/>
-      <c r="R28" s="118"/>
-      <c r="S28" s="118"/>
-      <c r="T28" s="118"/>
-      <c r="U28" s="118"/>
-      <c r="V28" s="118"/>
-      <c r="W28" s="83"/>
+      <c r="L28" s="109"/>
+      <c r="M28" s="110"/>
+      <c r="N28" s="110"/>
+      <c r="O28" s="110"/>
+      <c r="P28" s="111"/>
+      <c r="Q28" s="111"/>
+      <c r="R28" s="111"/>
+      <c r="S28" s="111"/>
+      <c r="T28" s="111"/>
+      <c r="U28" s="111"/>
+      <c r="V28" s="111"/>
+      <c r="W28" s="77"/>
       <c r="X28" s="23"/>
-      <c r="AB28" s="86"/>
+      <c r="AB28" s="80"/>
     </row>
     <row r="29" spans="2:35" s="17" customFormat="1">
       <c r="B29" s="22"/>
@@ -2380,40 +2407,40 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="K29" s="31"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="117"/>
-      <c r="N29" s="117"/>
-      <c r="O29" s="117"/>
-      <c r="P29" s="118"/>
-      <c r="Q29" s="118"/>
-      <c r="R29" s="118"/>
-      <c r="S29" s="118"/>
-      <c r="T29" s="118"/>
-      <c r="U29" s="118"/>
-      <c r="V29" s="118"/>
-      <c r="W29" s="83"/>
+      <c r="L29" s="109"/>
+      <c r="M29" s="110"/>
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="111"/>
+      <c r="Q29" s="111"/>
+      <c r="R29" s="111"/>
+      <c r="S29" s="111"/>
+      <c r="T29" s="111"/>
+      <c r="U29" s="111"/>
+      <c r="V29" s="111"/>
+      <c r="W29" s="77"/>
       <c r="X29" s="23"/>
     </row>
     <row r="30" spans="2:35" s="17" customFormat="1">
       <c r="B30" s="22"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="117"/>
-      <c r="N30" s="117"/>
-      <c r="O30" s="117"/>
-      <c r="P30" s="118"/>
-      <c r="Q30" s="118"/>
-      <c r="R30" s="118"/>
-      <c r="S30" s="118"/>
-      <c r="T30" s="118"/>
-      <c r="U30" s="118"/>
-      <c r="V30" s="118"/>
-      <c r="W30" s="83"/>
+      <c r="L30" s="109"/>
+      <c r="M30" s="110"/>
+      <c r="N30" s="110"/>
+      <c r="O30" s="110"/>
+      <c r="P30" s="111"/>
+      <c r="Q30" s="111"/>
+      <c r="R30" s="111"/>
+      <c r="S30" s="111"/>
+      <c r="T30" s="111"/>
+      <c r="U30" s="111"/>
+      <c r="V30" s="111"/>
+      <c r="W30" s="77"/>
       <c r="X30" s="23"/>
     </row>
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
       <c r="C31" s="39" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2423,18 +2450,18 @@
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
-      <c r="L31" s="119"/>
-      <c r="M31" s="117"/>
-      <c r="N31" s="117"/>
-      <c r="O31" s="117"/>
-      <c r="P31" s="118"/>
-      <c r="Q31" s="118"/>
-      <c r="R31" s="118"/>
-      <c r="S31" s="118"/>
-      <c r="T31" s="118"/>
-      <c r="U31" s="118"/>
-      <c r="V31" s="118"/>
-      <c r="W31" s="83"/>
+      <c r="L31" s="112"/>
+      <c r="M31" s="110"/>
+      <c r="N31" s="110"/>
+      <c r="O31" s="110"/>
+      <c r="P31" s="111"/>
+      <c r="Q31" s="111"/>
+      <c r="R31" s="111"/>
+      <c r="S31" s="111"/>
+      <c r="T31" s="111"/>
+      <c r="U31" s="111"/>
+      <c r="V31" s="111"/>
+      <c r="W31" s="77"/>
       <c r="X31" s="23"/>
       <c r="AA31" s="17"/>
       <c r="AB31" s="17"/>
@@ -2449,7 +2476,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2459,18 +2486,18 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
-      <c r="L32" s="116"/>
-      <c r="M32" s="117"/>
-      <c r="N32" s="117"/>
-      <c r="O32" s="117"/>
-      <c r="P32" s="118"/>
-      <c r="Q32" s="118"/>
-      <c r="R32" s="118"/>
-      <c r="S32" s="118"/>
-      <c r="T32" s="118"/>
-      <c r="U32" s="118"/>
-      <c r="V32" s="118"/>
-      <c r="W32" s="83"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
+      <c r="O32" s="110"/>
+      <c r="P32" s="111"/>
+      <c r="Q32" s="111"/>
+      <c r="R32" s="111"/>
+      <c r="S32" s="111"/>
+      <c r="T32" s="111"/>
+      <c r="U32" s="111"/>
+      <c r="V32" s="111"/>
+      <c r="W32" s="77"/>
       <c r="X32" s="23"/>
       <c r="AA32" s="17"/>
       <c r="AB32" s="17"/>
@@ -2493,18 +2520,18 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="116"/>
-      <c r="M33" s="120"/>
-      <c r="N33" s="117"/>
-      <c r="O33" s="117"/>
-      <c r="P33" s="118"/>
-      <c r="Q33" s="118"/>
-      <c r="R33" s="118"/>
-      <c r="S33" s="118"/>
-      <c r="T33" s="118"/>
-      <c r="U33" s="118"/>
-      <c r="V33" s="121"/>
-      <c r="W33" s="84"/>
+      <c r="L33" s="109"/>
+      <c r="M33" s="113"/>
+      <c r="N33" s="110"/>
+      <c r="O33" s="110"/>
+      <c r="P33" s="111"/>
+      <c r="Q33" s="111"/>
+      <c r="R33" s="111"/>
+      <c r="S33" s="111"/>
+      <c r="T33" s="111"/>
+      <c r="U33" s="111"/>
+      <c r="V33" s="114"/>
+      <c r="W33" s="78"/>
       <c r="X33" s="23"/>
       <c r="AA33" s="17"/>
       <c r="AB33" s="17"/>
@@ -2519,7 +2546,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2543,7 +2570,7 @@
       <c r="W34" s="45"/>
       <c r="X34" s="23"/>
       <c r="AA34" s="17"/>
-      <c r="AB34" s="86"/>
+      <c r="AB34" s="80"/>
       <c r="AC34" s="17"/>
       <c r="AD34" s="17"/>
       <c r="AE34" s="17"/>
@@ -2555,7 +2582,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2820,10 +2847,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B28" sqref="B28:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2835,1274 +2862,1410 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="65" customFormat="1">
-      <c r="A1" s="87" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="88" t="str">
+    <row r="1" spans="1:11" s="62" customFormat="1">
+      <c r="A1" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="82" t="str">
         <f>Overview!E9</f>
         <v>Hear and Note</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="90" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="91" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="104">
+        <f>COUNTIF(H1:H791,"OK")</f>
+        <v>3</v>
+      </c>
+      <c r="J1" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="87"/>
+    </row>
+    <row r="2" spans="1:11" s="62" customFormat="1">
+      <c r="A2" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="111">
-        <f>COUNTIF(H1:H786,"OK")</f>
-        <v>1</v>
-      </c>
-      <c r="J1" s="92" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="93"/>
-    </row>
-    <row r="2" spans="1:11" s="65" customFormat="1">
-      <c r="A2" s="126" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="95" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="98" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="112">
-        <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>4</v>
-      </c>
-      <c r="J2" s="99" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="100"/>
-    </row>
-    <row r="3" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A3" s="94" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="95" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="98" t="s">
+      <c r="B2" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="105">
+        <f>COUNTIF(H2:H792,"Not OK")</f>
+        <v>3</v>
+      </c>
+      <c r="J2" s="93" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="94"/>
+    </row>
+    <row r="3" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A3" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="106">
+        <f>COUNTIF(H2:H792,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="94"/>
+    </row>
+    <row r="4" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A4" s="95"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="89"/>
+      <c r="I4" s="105">
+        <f>COUNTIF(H3:H793,"Result")</f>
+        <v>6</v>
+      </c>
+      <c r="J4" s="93"/>
+      <c r="K4" s="94"/>
+    </row>
+    <row r="5" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="102"/>
+    </row>
+    <row r="6" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A6" s="63"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+    </row>
+    <row r="7" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A7" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="147" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="113">
-        <f>COUNTIF(H2:H787,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="99" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="100"/>
-    </row>
-    <row r="4" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A4" s="101"/>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="102" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="95"/>
-      <c r="I4" s="112">
-        <f>COUNTIF(H3:H788,"Result")</f>
-        <v>5</v>
-      </c>
-      <c r="J4" s="99"/>
-      <c r="K4" s="100"/>
-    </row>
-    <row r="5" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="108"/>
-    </row>
-    <row r="6" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A6" s="69"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-    </row>
-    <row r="7" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A7" s="109" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="129" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="147"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="132" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="133"/>
-      <c r="F8" s="132" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="133"/>
-      <c r="H8" s="131" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="131"/>
+        <v>22</v>
+      </c>
+      <c r="B8" s="122" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="123"/>
+      <c r="D8" s="122" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="123"/>
+      <c r="F8" s="122" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="123"/>
+      <c r="H8" s="148" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="148"/>
       <c r="J8" s="48" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K8" s="49" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="151" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="152"/>
-      <c r="D9" s="142" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="66"/>
+      <c r="B9" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="126"/>
+      <c r="D9" s="134" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="135"/>
+      <c r="F9" s="134" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="135"/>
       <c r="H9" s="140" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I9" s="141"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="137"/>
+      <c r="K9" s="144"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="153"/>
-      <c r="C10" s="154"/>
-      <c r="D10" s="144"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="67"/>
+        <v>28</v>
+      </c>
+      <c r="B10" s="127"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="137"/>
       <c r="H10" s="47" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="138"/>
+        <v>34</v>
+      </c>
+      <c r="K10" s="145"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A11" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="153"/>
-      <c r="C11" s="154"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="54"/>
+      <c r="A11" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="127"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="52"/>
       <c r="J11" s="50"/>
-      <c r="K11" s="138"/>
+      <c r="K11" s="145"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="67"/>
+      <c r="B12" s="127"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="137"/>
       <c r="H12" s="47" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I12" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="47"/>
+      <c r="K12" s="145"/>
+    </row>
+    <row r="13" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A13" s="53">
+        <v>981</v>
+      </c>
+      <c r="B13" s="129"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="146"/>
+    </row>
+    <row r="14" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A14" s="153" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="154" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="155"/>
+      <c r="D14" s="154" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="155"/>
+      <c r="F14" s="154" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="155"/>
+      <c r="H14" s="156" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="156"/>
+      <c r="J14" s="157" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="158" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A15" s="150">
+        <v>2</v>
+      </c>
+      <c r="B15" s="159" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="160"/>
+      <c r="D15" s="134" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="135"/>
+      <c r="F15" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="135"/>
+      <c r="H15" s="151" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="152"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="144"/>
+    </row>
+    <row r="16" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A16" s="153" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="161"/>
+      <c r="C16" s="162"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="137"/>
+      <c r="H16" s="165" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="165" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="166" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="145"/>
+    </row>
+    <row r="17" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A17" s="150" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="161"/>
+      <c r="C17" s="162"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="145"/>
+    </row>
+    <row r="18" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A18" s="153" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="161"/>
+      <c r="C18" s="162"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="165" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="165" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="166"/>
+      <c r="K18" s="145"/>
+    </row>
+    <row r="19" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A19" s="150">
+        <v>933</v>
+      </c>
+      <c r="B19" s="163"/>
+      <c r="C19" s="164"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="55"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="146"/>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A20" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="133"/>
+      <c r="D20" s="132" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="133"/>
+      <c r="F20" s="132" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="133"/>
+      <c r="H20" s="131" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="131"/>
+      <c r="J20" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A21" s="50">
+        <v>3</v>
+      </c>
+      <c r="B21" s="125" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="126"/>
+      <c r="D21" s="134" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="135"/>
+      <c r="F21" s="134" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="135"/>
+      <c r="H21" s="142" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="143"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="144"/>
+    </row>
+    <row r="22" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A22" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="127"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="136"/>
+      <c r="G22" s="137"/>
+      <c r="H22" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="145"/>
+    </row>
+    <row r="23" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A23" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="127"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="137"/>
+      <c r="H23" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" s="52"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="145"/>
+    </row>
+    <row r="24" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A24" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="127"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="136"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="59"/>
+      <c r="K24" s="145"/>
+    </row>
+    <row r="25" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A25" s="53">
+        <v>921</v>
+      </c>
+      <c r="B25" s="129"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" s="52"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="145"/>
+    </row>
+    <row r="26" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A26" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="149" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="149"/>
+      <c r="D26" s="147"/>
+      <c r="E26" s="147"/>
+      <c r="F26" s="147"/>
+      <c r="G26" s="147"/>
+      <c r="H26" s="147"/>
+      <c r="I26" s="147"/>
+      <c r="J26" s="147"/>
+      <c r="K26" s="147"/>
+    </row>
+    <row r="27" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A27" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="133"/>
+      <c r="D27" s="132" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="133"/>
+      <c r="F27" s="132" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="133"/>
+      <c r="H27" s="131" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="131"/>
+      <c r="J27" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A28" s="50">
+        <f>A21+1</f>
+        <v>4</v>
+      </c>
+      <c r="B28" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="126"/>
+      <c r="D28" s="134" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="135"/>
+      <c r="F28" s="134" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="135"/>
+      <c r="H28" s="140" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="141"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="144"/>
+    </row>
+    <row r="29" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A29" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="127"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="137"/>
+      <c r="F29" s="136"/>
+      <c r="G29" s="137"/>
+      <c r="H29" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="145"/>
+    </row>
+    <row r="30" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A30" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="127"/>
+      <c r="C30" s="128"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" s="52"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="145"/>
+    </row>
+    <row r="31" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A31" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="127"/>
+      <c r="C31" s="128"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="145"/>
+    </row>
+    <row r="32" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A32" s="53">
+        <v>922</v>
+      </c>
+      <c r="B32" s="129"/>
+      <c r="C32" s="130"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="139"/>
+      <c r="H32" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" s="52"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="146"/>
+    </row>
+    <row r="33" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A33" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="122" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="123"/>
+      <c r="D33" s="122" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="123"/>
+      <c r="F33" s="122" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="123"/>
+      <c r="H33" s="124" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="124"/>
+      <c r="J33" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A34" s="50">
+        <v>4</v>
+      </c>
+      <c r="B34" s="125" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="126"/>
+      <c r="D34" s="134" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="135"/>
+      <c r="F34" s="134" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="135"/>
+      <c r="H34" s="142" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="143"/>
+      <c r="J34" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" s="144"/>
+    </row>
+    <row r="35" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A35" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="127"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="136"/>
+      <c r="E35" s="137"/>
+      <c r="F35" s="136"/>
+      <c r="G35" s="137"/>
+      <c r="H35" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" s="145"/>
+    </row>
+    <row r="36" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A36" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="127"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="136"/>
+      <c r="G36" s="137"/>
+      <c r="H36" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="47"/>
-      <c r="K12" s="138"/>
-    </row>
-    <row r="13" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A13" s="55">
-        <v>981</v>
-      </c>
-      <c r="B13" s="155"/>
-      <c r="C13" s="156"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="147"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="58" t="s">
+      <c r="J36" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="K36" s="145"/>
+    </row>
+    <row r="37" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A37" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="127"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="137"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="137"/>
+      <c r="H37" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" s="47"/>
+      <c r="K37" s="145"/>
+    </row>
+    <row r="38" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A38" s="53">
+        <v>823</v>
+      </c>
+      <c r="B38" s="129"/>
+      <c r="C38" s="130"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="139"/>
+      <c r="F38" s="138"/>
+      <c r="G38" s="139"/>
+      <c r="H38" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I38" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="J38" s="50"/>
+      <c r="K38" s="146"/>
+    </row>
+    <row r="39" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A39" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="122" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="123"/>
+      <c r="D39" s="122" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="123"/>
+      <c r="F39" s="122" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="123"/>
+      <c r="H39" s="124" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" s="124"/>
+      <c r="J39" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K39" s="60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A40" s="50">
+        <v>5</v>
+      </c>
+      <c r="B40" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="58"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="139"/>
-    </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A14" s="60" t="s">
+      <c r="C40" s="126"/>
+      <c r="D40" s="134" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="135"/>
+      <c r="F40" s="134" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="135"/>
+      <c r="H40" s="142" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="143"/>
+      <c r="J40" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="K40" s="144"/>
+    </row>
+    <row r="41" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A41" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="135" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="136"/>
-      <c r="D14" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="136"/>
-      <c r="F14" s="135" t="s">
+      <c r="B41" s="127"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="137"/>
+      <c r="F41" s="136"/>
+      <c r="G41" s="137"/>
+      <c r="H41" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="136"/>
-      <c r="H14" s="150" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="150"/>
-      <c r="J14" s="62" t="s">
+      <c r="I41" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" s="145"/>
+    </row>
+    <row r="42" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A42" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="127"/>
+      <c r="C42" s="128"/>
+      <c r="D42" s="136"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="136"/>
+      <c r="G42" s="137"/>
+      <c r="H42" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="61" t="s">
+      <c r="K42" s="145"/>
+    </row>
+    <row r="43" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A43" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="127"/>
+      <c r="C43" s="128"/>
+      <c r="D43" s="136"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="136"/>
+      <c r="G43" s="137"/>
+      <c r="H43" s="47" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A15" s="50">
+      <c r="I43" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="J43" s="47"/>
+      <c r="K43" s="145"/>
+    </row>
+    <row r="44" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A44" s="53">
+        <v>823</v>
+      </c>
+      <c r="B44" s="129"/>
+      <c r="C44" s="130"/>
+      <c r="D44" s="138"/>
+      <c r="E44" s="139"/>
+      <c r="F44" s="138"/>
+      <c r="G44" s="139"/>
+      <c r="H44" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I44" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="151" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="152"/>
-      <c r="D15" s="142" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="143"/>
-      <c r="F15" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="66"/>
-      <c r="H15" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I15" s="158"/>
-      <c r="J15" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="137"/>
-    </row>
-    <row r="16" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A16" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="145"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="138"/>
-    </row>
-    <row r="17" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A17" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="154"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" s="138"/>
-    </row>
-    <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="153"/>
-      <c r="C18" s="154"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="J18" s="62"/>
-      <c r="K18" s="138"/>
-    </row>
-    <row r="19" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A19" s="55">
-        <v>921</v>
-      </c>
-      <c r="B19" s="155"/>
-      <c r="C19" s="156"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="147"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="50"/>
-      <c r="K19" s="138"/>
-    </row>
-    <row r="20" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A20" s="109" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="134" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="129"/>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
-      <c r="J20" s="129"/>
-      <c r="K20" s="129"/>
-    </row>
-    <row r="21" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A21" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="148" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="148"/>
-      <c r="D21" s="149"/>
-      <c r="E21" s="149"/>
-      <c r="F21" s="149"/>
-      <c r="G21" s="149"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="149"/>
-      <c r="J21" s="149"/>
-      <c r="K21" s="149"/>
-    </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A22" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="135" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="136"/>
-      <c r="D22" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="136"/>
-      <c r="F22" s="135" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="136"/>
-      <c r="H22" s="150" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="150"/>
-      <c r="J22" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="62" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A23" s="50">
-        <f>A15+1</f>
-        <v>3</v>
-      </c>
-      <c r="B23" s="151" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="152"/>
-      <c r="D23" s="142" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="143"/>
-      <c r="F23" s="142" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="143"/>
-      <c r="H23" s="140" t="s">
-        <v>37</v>
-      </c>
-      <c r="I23" s="141"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="137"/>
-    </row>
-    <row r="24" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A24" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="153"/>
-      <c r="C24" s="154"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" s="138"/>
-    </row>
-    <row r="25" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A25" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="153"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I25" s="54"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="138"/>
-    </row>
-    <row r="26" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A26" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="153"/>
-      <c r="C26" s="154"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="145"/>
-      <c r="H26" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="138"/>
-    </row>
-    <row r="27" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A27" s="55">
-        <v>922</v>
-      </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="156"/>
-      <c r="D27" s="146"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="146"/>
-      <c r="G27" s="147"/>
-      <c r="H27" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="139"/>
-    </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A28" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="132" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="133"/>
-      <c r="D28" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="133"/>
-      <c r="F28" s="132" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28" s="133"/>
-      <c r="H28" s="130" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="130"/>
-      <c r="J28" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="63" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A29" s="50">
-        <v>4</v>
-      </c>
-      <c r="B29" s="151" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="142" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="143"/>
-      <c r="F29" s="142" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="143"/>
-      <c r="H29" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29" s="158"/>
-      <c r="J29" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="K29" s="137"/>
-    </row>
-    <row r="30" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A30" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="153"/>
-      <c r="C30" s="154"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="145"/>
-      <c r="H30" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I30" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="J30" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="138"/>
-    </row>
-    <row r="31" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A31" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="153"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J31" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="138"/>
-    </row>
-    <row r="32" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A32" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="153"/>
-      <c r="C32" s="154"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="145"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="145"/>
-      <c r="H32" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="J32" s="47"/>
-      <c r="K32" s="138"/>
-    </row>
-    <row r="33" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A33" s="55">
-        <v>823</v>
-      </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="156"/>
-      <c r="D33" s="146"/>
-      <c r="E33" s="147"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="147"/>
-      <c r="H33" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I33" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="J33" s="50"/>
-      <c r="K33" s="139"/>
-    </row>
-    <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A34" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="132" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="133"/>
-      <c r="D34" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="133"/>
-      <c r="F34" s="132" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" s="133"/>
-      <c r="H34" s="130" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="130"/>
-      <c r="J34" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="K34" s="63" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A35" s="50">
-        <v>5</v>
-      </c>
-      <c r="B35" s="151" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="152"/>
-      <c r="D35" s="142" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="143"/>
-      <c r="F35" s="142" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" s="143"/>
-      <c r="H35" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I35" s="158"/>
-      <c r="J35" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="K35" s="137"/>
-    </row>
-    <row r="36" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A36" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="153"/>
-      <c r="C36" s="154"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I36" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="J36" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="138"/>
-    </row>
-    <row r="37" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A37" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="153"/>
-      <c r="C37" s="154"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="K37" s="138"/>
-    </row>
-    <row r="38" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A38" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="153"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="145"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="145"/>
-      <c r="H38" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="I38" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="J38" s="47"/>
-      <c r="K38" s="138"/>
-    </row>
-    <row r="39" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A39" s="55">
-        <v>823</v>
-      </c>
-      <c r="B39" s="155"/>
-      <c r="C39" s="156"/>
-      <c r="D39" s="146"/>
-      <c r="E39" s="147"/>
-      <c r="F39" s="146"/>
-      <c r="G39" s="147"/>
-      <c r="H39" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="J39" s="50"/>
-      <c r="K39" s="139"/>
-    </row>
-    <row r="40" spans="1:11" s="65" customFormat="1">
-      <c r="A40" s="72"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-    </row>
-    <row r="41" spans="1:11" s="65" customFormat="1">
-      <c r="A41" s="72"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="72"/>
-    </row>
-    <row r="42" spans="1:11" s="65" customFormat="1">
-      <c r="A42" s="72"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-    </row>
-    <row r="43" spans="1:11" s="65" customFormat="1">
-      <c r="A43" s="72"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="72"/>
-    </row>
-    <row r="44" spans="1:11" s="65" customFormat="1">
-      <c r="A44" s="72"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
-      <c r="K44" s="72"/>
-    </row>
-    <row r="45" spans="1:11" s="65" customFormat="1">
-      <c r="A45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
-      <c r="K45" s="72"/>
-    </row>
-    <row r="46" spans="1:11" s="65" customFormat="1">
-      <c r="A46" s="72"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="72"/>
-      <c r="J46" s="72"/>
-      <c r="K46" s="72"/>
-    </row>
-    <row r="47" spans="1:11" s="65" customFormat="1">
-      <c r="A47" s="72"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="72"/>
-    </row>
-    <row r="48" spans="1:11" s="65" customFormat="1">
-      <c r="A48" s="72"/>
-      <c r="H48" s="72"/>
-      <c r="I48" s="72"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="72"/>
-    </row>
-    <row r="49" spans="1:11" s="65" customFormat="1">
-      <c r="A49" s="72"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="72"/>
-      <c r="K49" s="72"/>
-    </row>
-    <row r="50" spans="1:11" s="65" customFormat="1">
-      <c r="A50" s="72"/>
-      <c r="H50" s="72"/>
-      <c r="I50" s="72"/>
-      <c r="J50" s="72"/>
-      <c r="K50" s="72"/>
-    </row>
-    <row r="51" spans="1:11" s="65" customFormat="1">
-      <c r="A51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="72"/>
-    </row>
-    <row r="52" spans="1:11" s="65" customFormat="1">
-      <c r="A52" s="72"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="72"/>
-      <c r="K52" s="72"/>
-    </row>
-    <row r="53" spans="1:11" s="65" customFormat="1">
-      <c r="A53" s="72"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="72"/>
-      <c r="J53" s="72"/>
-      <c r="K53" s="72"/>
-    </row>
-    <row r="54" spans="1:11" s="65" customFormat="1">
-      <c r="A54" s="72"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
-      <c r="K54" s="72"/>
-    </row>
-    <row r="55" spans="1:11" s="65" customFormat="1">
-      <c r="A55" s="72"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="72"/>
-      <c r="J55" s="72"/>
-      <c r="K55" s="72"/>
-    </row>
-    <row r="56" spans="1:11" s="65" customFormat="1">
-      <c r="A56" s="72"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="72"/>
-      <c r="K56" s="72"/>
-    </row>
-    <row r="57" spans="1:11" s="65" customFormat="1">
-      <c r="A57" s="72"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="72"/>
-      <c r="K57" s="72"/>
-    </row>
-    <row r="58" spans="1:11" s="65" customFormat="1">
-      <c r="A58" s="72"/>
-      <c r="H58" s="72"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="72"/>
-      <c r="K58" s="72"/>
-    </row>
-    <row r="59" spans="1:11" s="65" customFormat="1">
-      <c r="A59" s="72"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="72"/>
-      <c r="K59" s="72"/>
-    </row>
-    <row r="60" spans="1:11" s="65" customFormat="1">
-      <c r="A60" s="72"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="72"/>
-      <c r="J60" s="72"/>
-      <c r="K60" s="72"/>
-    </row>
-    <row r="61" spans="1:11" s="65" customFormat="1">
-      <c r="A61" s="72"/>
-      <c r="H61" s="72"/>
-      <c r="I61" s="72"/>
-      <c r="J61" s="72"/>
-      <c r="K61" s="72"/>
-    </row>
-    <row r="62" spans="1:11" s="65" customFormat="1">
-      <c r="A62" s="72"/>
-      <c r="H62" s="72"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="72"/>
-    </row>
-    <row r="63" spans="1:11" s="65" customFormat="1">
-      <c r="A63" s="72"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="72"/>
-      <c r="J63" s="72"/>
-      <c r="K63" s="72"/>
-    </row>
-    <row r="64" spans="1:11" s="65" customFormat="1">
-      <c r="A64" s="72"/>
-      <c r="H64" s="72"/>
-      <c r="I64" s="72"/>
-      <c r="J64" s="72"/>
-      <c r="K64" s="72"/>
-    </row>
-    <row r="65" spans="1:11" s="65" customFormat="1">
-      <c r="A65" s="72"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
-      <c r="J65" s="72"/>
-      <c r="K65" s="72"/>
-    </row>
-    <row r="66" spans="1:11" s="65" customFormat="1">
-      <c r="A66" s="72"/>
-      <c r="H66" s="72"/>
-      <c r="I66" s="72"/>
-      <c r="J66" s="72"/>
-      <c r="K66" s="72"/>
-    </row>
-    <row r="67" spans="1:11" s="65" customFormat="1">
-      <c r="A67" s="72"/>
-      <c r="H67" s="72"/>
-      <c r="I67" s="72"/>
-      <c r="J67" s="72"/>
-      <c r="K67" s="72"/>
-    </row>
-    <row r="68" spans="1:11" s="65" customFormat="1">
-      <c r="A68" s="72"/>
-      <c r="H68" s="72"/>
-      <c r="I68" s="72"/>
-      <c r="J68" s="72"/>
-      <c r="K68" s="72"/>
-    </row>
-    <row r="69" spans="1:11" s="65" customFormat="1">
-      <c r="A69" s="72"/>
-      <c r="H69" s="72"/>
-      <c r="I69" s="72"/>
-      <c r="J69" s="72"/>
-      <c r="K69" s="72"/>
-    </row>
-    <row r="70" spans="1:11" s="65" customFormat="1">
-      <c r="A70" s="72"/>
-      <c r="H70" s="72"/>
-      <c r="I70" s="72"/>
-      <c r="J70" s="72"/>
-      <c r="K70" s="72"/>
-    </row>
-    <row r="71" spans="1:11" s="65" customFormat="1">
-      <c r="A71" s="72"/>
-      <c r="H71" s="72"/>
-      <c r="I71" s="72"/>
-      <c r="J71" s="72"/>
-      <c r="K71" s="72"/>
-    </row>
-    <row r="72" spans="1:11" s="65" customFormat="1">
-      <c r="A72" s="72"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="72"/>
-      <c r="J72" s="72"/>
-      <c r="K72" s="72"/>
-    </row>
-    <row r="73" spans="1:11" s="65" customFormat="1">
-      <c r="A73" s="72"/>
-      <c r="H73" s="72"/>
-      <c r="I73" s="72"/>
-      <c r="J73" s="72"/>
-      <c r="K73" s="72"/>
-    </row>
-    <row r="74" spans="1:11" s="65" customFormat="1">
-      <c r="A74" s="72"/>
-      <c r="H74" s="72"/>
-      <c r="I74" s="72"/>
-      <c r="J74" s="72"/>
-      <c r="K74" s="72"/>
-    </row>
-    <row r="75" spans="1:11" s="65" customFormat="1">
-      <c r="A75" s="72"/>
-      <c r="H75" s="72"/>
-      <c r="I75" s="72"/>
-      <c r="J75" s="72"/>
-      <c r="K75" s="72"/>
-    </row>
-    <row r="76" spans="1:11" s="65" customFormat="1">
-      <c r="A76" s="72"/>
-      <c r="H76" s="72"/>
-      <c r="I76" s="72"/>
-      <c r="J76" s="72"/>
-      <c r="K76" s="72"/>
-    </row>
-    <row r="77" spans="1:11" s="65" customFormat="1">
-      <c r="A77" s="72"/>
-      <c r="H77" s="72"/>
-      <c r="I77" s="72"/>
-      <c r="J77" s="72"/>
-      <c r="K77" s="72"/>
-    </row>
-    <row r="78" spans="1:11" s="65" customFormat="1">
-      <c r="A78" s="72"/>
-      <c r="H78" s="72"/>
-      <c r="I78" s="72"/>
-      <c r="J78" s="72"/>
-      <c r="K78" s="72"/>
-    </row>
-    <row r="79" spans="1:11" s="65" customFormat="1">
-      <c r="A79" s="72"/>
-      <c r="H79" s="72"/>
-      <c r="I79" s="72"/>
-      <c r="J79" s="72"/>
-      <c r="K79" s="72"/>
-    </row>
-    <row r="80" spans="1:11" s="65" customFormat="1">
-      <c r="A80" s="72"/>
-      <c r="H80" s="72"/>
-      <c r="I80" s="72"/>
-      <c r="J80" s="72"/>
-      <c r="K80" s="72"/>
-    </row>
-    <row r="81" spans="1:11" s="65" customFormat="1">
-      <c r="A81" s="72"/>
-      <c r="H81" s="72"/>
-      <c r="I81" s="72"/>
-      <c r="J81" s="72"/>
-      <c r="K81" s="72"/>
-    </row>
-    <row r="82" spans="1:11" s="65" customFormat="1">
-      <c r="A82" s="72"/>
-      <c r="H82" s="72"/>
-      <c r="I82" s="72"/>
-      <c r="J82" s="72"/>
-      <c r="K82" s="72"/>
-    </row>
-    <row r="83" spans="1:11" s="65" customFormat="1">
-      <c r="A83" s="72"/>
-      <c r="H83" s="72"/>
-      <c r="I83" s="72"/>
-      <c r="J83" s="72"/>
-      <c r="K83" s="72"/>
-    </row>
-    <row r="84" spans="1:11" s="65" customFormat="1">
-      <c r="A84" s="72"/>
-      <c r="H84" s="72"/>
-      <c r="I84" s="72"/>
-      <c r="J84" s="72"/>
-      <c r="K84" s="72"/>
-    </row>
-    <row r="85" spans="1:11" s="65" customFormat="1">
-      <c r="A85" s="72"/>
-      <c r="H85" s="72"/>
-      <c r="I85" s="72"/>
-      <c r="J85" s="72"/>
-      <c r="K85" s="72"/>
-    </row>
-    <row r="86" spans="1:11" s="65" customFormat="1">
-      <c r="A86" s="72"/>
-      <c r="H86" s="72"/>
-      <c r="I86" s="72"/>
-      <c r="J86" s="72"/>
-      <c r="K86" s="72"/>
-    </row>
-    <row r="87" spans="1:11" s="65" customFormat="1">
-      <c r="A87" s="72"/>
-      <c r="H87" s="72"/>
-      <c r="I87" s="72"/>
-      <c r="J87" s="72"/>
-      <c r="K87" s="72"/>
-    </row>
-    <row r="88" spans="1:11" s="65" customFormat="1">
-      <c r="A88" s="72"/>
-      <c r="H88" s="72"/>
-      <c r="I88" s="72"/>
-      <c r="J88" s="72"/>
-      <c r="K88" s="72"/>
-    </row>
-    <row r="89" spans="1:11" s="65" customFormat="1">
-      <c r="A89" s="72"/>
-      <c r="H89" s="72"/>
-      <c r="I89" s="72"/>
-      <c r="J89" s="72"/>
-      <c r="K89" s="72"/>
-    </row>
-    <row r="90" spans="1:11" s="65" customFormat="1">
-      <c r="A90" s="72"/>
-      <c r="H90" s="72"/>
-      <c r="I90" s="72"/>
-      <c r="J90" s="72"/>
-      <c r="K90" s="72"/>
-    </row>
-    <row r="91" spans="1:11" s="65" customFormat="1">
-      <c r="A91" s="72"/>
-      <c r="H91" s="72"/>
-      <c r="I91" s="72"/>
-      <c r="J91" s="72"/>
-      <c r="K91" s="72"/>
-    </row>
-    <row r="92" spans="1:11" s="65" customFormat="1">
-      <c r="A92" s="72"/>
-      <c r="H92" s="72"/>
-      <c r="I92" s="72"/>
-      <c r="J92" s="72"/>
-      <c r="K92" s="72"/>
-    </row>
-    <row r="93" spans="1:11" s="65" customFormat="1">
-      <c r="A93" s="72"/>
-      <c r="H93" s="72"/>
-      <c r="I93" s="72"/>
-      <c r="J93" s="72"/>
-      <c r="K93" s="72"/>
-    </row>
-    <row r="94" spans="1:11" s="65" customFormat="1">
-      <c r="A94" s="72"/>
-      <c r="H94" s="72"/>
-      <c r="I94" s="72"/>
-      <c r="J94" s="72"/>
-      <c r="K94" s="72"/>
-    </row>
-    <row r="95" spans="1:11" s="65" customFormat="1">
-      <c r="A95" s="72"/>
-      <c r="H95" s="72"/>
-      <c r="I95" s="72"/>
-      <c r="J95" s="72"/>
-      <c r="K95" s="72"/>
-    </row>
-    <row r="96" spans="1:11" s="65" customFormat="1">
-      <c r="A96" s="72"/>
-      <c r="H96" s="72"/>
-      <c r="I96" s="72"/>
-      <c r="J96" s="72"/>
-      <c r="K96" s="72"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="146"/>
+    </row>
+    <row r="45" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A45" s="66"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="66"/>
+      <c r="I45" s="66"/>
+      <c r="J45" s="66"/>
+      <c r="K45" s="66"/>
+    </row>
+    <row r="46" spans="1:11" s="62" customFormat="1">
+      <c r="A46" s="66"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="66"/>
+    </row>
+    <row r="47" spans="1:11" s="62" customFormat="1">
+      <c r="A47" s="66"/>
+      <c r="H47" s="66"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="66"/>
+    </row>
+    <row r="48" spans="1:11" s="62" customFormat="1">
+      <c r="A48" s="66"/>
+      <c r="H48" s="66"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="66"/>
+      <c r="K48" s="66"/>
+    </row>
+    <row r="49" spans="1:11" s="62" customFormat="1">
+      <c r="A49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="66"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="66"/>
+    </row>
+    <row r="50" spans="1:11" s="62" customFormat="1">
+      <c r="A50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
+    </row>
+    <row r="51" spans="1:11" s="62" customFormat="1">
+      <c r="A51" s="66"/>
+      <c r="H51" s="66"/>
+      <c r="I51" s="66"/>
+      <c r="J51" s="66"/>
+      <c r="K51" s="66"/>
+    </row>
+    <row r="52" spans="1:11" s="62" customFormat="1">
+      <c r="A52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="66"/>
+    </row>
+    <row r="53" spans="1:11" s="62" customFormat="1">
+      <c r="A53" s="66"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="66"/>
+      <c r="J53" s="66"/>
+      <c r="K53" s="66"/>
+    </row>
+    <row r="54" spans="1:11" s="62" customFormat="1">
+      <c r="A54" s="66"/>
+      <c r="H54" s="66"/>
+      <c r="I54" s="66"/>
+      <c r="J54" s="66"/>
+      <c r="K54" s="66"/>
+    </row>
+    <row r="55" spans="1:11" s="62" customFormat="1">
+      <c r="A55" s="66"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="66"/>
+      <c r="J55" s="66"/>
+      <c r="K55" s="66"/>
+    </row>
+    <row r="56" spans="1:11" s="62" customFormat="1">
+      <c r="A56" s="66"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="66"/>
+      <c r="J56" s="66"/>
+      <c r="K56" s="66"/>
+    </row>
+    <row r="57" spans="1:11" s="62" customFormat="1">
+      <c r="A57" s="66"/>
+      <c r="H57" s="66"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="66"/>
+      <c r="K57" s="66"/>
+    </row>
+    <row r="58" spans="1:11" s="62" customFormat="1">
+      <c r="A58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="66"/>
+    </row>
+    <row r="59" spans="1:11" s="62" customFormat="1">
+      <c r="A59" s="66"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="66"/>
+    </row>
+    <row r="60" spans="1:11" s="62" customFormat="1">
+      <c r="A60" s="66"/>
+      <c r="H60" s="66"/>
+      <c r="I60" s="66"/>
+      <c r="J60" s="66"/>
+      <c r="K60" s="66"/>
+    </row>
+    <row r="61" spans="1:11" s="62" customFormat="1">
+      <c r="A61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+    </row>
+    <row r="62" spans="1:11" s="62" customFormat="1">
+      <c r="A62" s="66"/>
+      <c r="H62" s="66"/>
+      <c r="I62" s="66"/>
+      <c r="J62" s="66"/>
+      <c r="K62" s="66"/>
+    </row>
+    <row r="63" spans="1:11" s="62" customFormat="1">
+      <c r="A63" s="66"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="66"/>
+      <c r="J63" s="66"/>
+      <c r="K63" s="66"/>
+    </row>
+    <row r="64" spans="1:11" s="62" customFormat="1">
+      <c r="A64" s="66"/>
+      <c r="H64" s="66"/>
+      <c r="I64" s="66"/>
+      <c r="J64" s="66"/>
+      <c r="K64" s="66"/>
+    </row>
+    <row r="65" spans="1:11" s="62" customFormat="1">
+      <c r="A65" s="66"/>
+      <c r="H65" s="66"/>
+      <c r="I65" s="66"/>
+      <c r="J65" s="66"/>
+      <c r="K65" s="66"/>
+    </row>
+    <row r="66" spans="1:11" s="62" customFormat="1">
+      <c r="A66" s="66"/>
+      <c r="H66" s="66"/>
+      <c r="I66" s="66"/>
+      <c r="J66" s="66"/>
+      <c r="K66" s="66"/>
+    </row>
+    <row r="67" spans="1:11" s="62" customFormat="1">
+      <c r="A67" s="66"/>
+      <c r="H67" s="66"/>
+      <c r="I67" s="66"/>
+      <c r="J67" s="66"/>
+      <c r="K67" s="66"/>
+    </row>
+    <row r="68" spans="1:11" s="62" customFormat="1">
+      <c r="A68" s="66"/>
+      <c r="H68" s="66"/>
+      <c r="I68" s="66"/>
+      <c r="J68" s="66"/>
+      <c r="K68" s="66"/>
+    </row>
+    <row r="69" spans="1:11" s="62" customFormat="1">
+      <c r="A69" s="66"/>
+      <c r="H69" s="66"/>
+      <c r="I69" s="66"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="66"/>
+    </row>
+    <row r="70" spans="1:11" s="62" customFormat="1">
+      <c r="A70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="66"/>
+      <c r="J70" s="66"/>
+      <c r="K70" s="66"/>
+    </row>
+    <row r="71" spans="1:11" s="62" customFormat="1">
+      <c r="A71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="66"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="66"/>
+    </row>
+    <row r="72" spans="1:11" s="62" customFormat="1">
+      <c r="A72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="66"/>
+      <c r="J72" s="66"/>
+      <c r="K72" s="66"/>
+    </row>
+    <row r="73" spans="1:11" s="62" customFormat="1">
+      <c r="A73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="66"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+    </row>
+    <row r="74" spans="1:11" s="62" customFormat="1">
+      <c r="A74" s="66"/>
+      <c r="H74" s="66"/>
+      <c r="I74" s="66"/>
+      <c r="J74" s="66"/>
+      <c r="K74" s="66"/>
+    </row>
+    <row r="75" spans="1:11" s="62" customFormat="1">
+      <c r="A75" s="66"/>
+      <c r="H75" s="66"/>
+      <c r="I75" s="66"/>
+      <c r="J75" s="66"/>
+      <c r="K75" s="66"/>
+    </row>
+    <row r="76" spans="1:11" s="62" customFormat="1">
+      <c r="A76" s="66"/>
+      <c r="H76" s="66"/>
+      <c r="I76" s="66"/>
+      <c r="J76" s="66"/>
+      <c r="K76" s="66"/>
+    </row>
+    <row r="77" spans="1:11" s="62" customFormat="1">
+      <c r="A77" s="66"/>
+      <c r="H77" s="66"/>
+      <c r="I77" s="66"/>
+      <c r="J77" s="66"/>
+      <c r="K77" s="66"/>
+    </row>
+    <row r="78" spans="1:11" s="62" customFormat="1">
+      <c r="A78" s="66"/>
+      <c r="H78" s="66"/>
+      <c r="I78" s="66"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="66"/>
+    </row>
+    <row r="79" spans="1:11" s="62" customFormat="1">
+      <c r="A79" s="66"/>
+      <c r="H79" s="66"/>
+      <c r="I79" s="66"/>
+      <c r="J79" s="66"/>
+      <c r="K79" s="66"/>
+    </row>
+    <row r="80" spans="1:11" s="62" customFormat="1">
+      <c r="A80" s="66"/>
+      <c r="H80" s="66"/>
+      <c r="I80" s="66"/>
+      <c r="J80" s="66"/>
+      <c r="K80" s="66"/>
+    </row>
+    <row r="81" spans="1:11" s="62" customFormat="1">
+      <c r="A81" s="66"/>
+      <c r="H81" s="66"/>
+      <c r="I81" s="66"/>
+      <c r="J81" s="66"/>
+      <c r="K81" s="66"/>
+    </row>
+    <row r="82" spans="1:11" s="62" customFormat="1">
+      <c r="A82" s="66"/>
+      <c r="H82" s="66"/>
+      <c r="I82" s="66"/>
+      <c r="J82" s="66"/>
+      <c r="K82" s="66"/>
+    </row>
+    <row r="83" spans="1:11" s="62" customFormat="1">
+      <c r="A83" s="66"/>
+      <c r="H83" s="66"/>
+      <c r="I83" s="66"/>
+      <c r="J83" s="66"/>
+      <c r="K83" s="66"/>
+    </row>
+    <row r="84" spans="1:11" s="62" customFormat="1">
+      <c r="A84" s="66"/>
+      <c r="H84" s="66"/>
+      <c r="I84" s="66"/>
+      <c r="J84" s="66"/>
+      <c r="K84" s="66"/>
+    </row>
+    <row r="85" spans="1:11" s="62" customFormat="1">
+      <c r="A85" s="66"/>
+      <c r="H85" s="66"/>
+      <c r="I85" s="66"/>
+      <c r="J85" s="66"/>
+      <c r="K85" s="66"/>
+    </row>
+    <row r="86" spans="1:11" s="62" customFormat="1">
+      <c r="A86" s="66"/>
+      <c r="H86" s="66"/>
+      <c r="I86" s="66"/>
+      <c r="J86" s="66"/>
+      <c r="K86" s="66"/>
+    </row>
+    <row r="87" spans="1:11" s="62" customFormat="1">
+      <c r="A87" s="66"/>
+      <c r="H87" s="66"/>
+      <c r="I87" s="66"/>
+      <c r="J87" s="66"/>
+      <c r="K87" s="66"/>
+    </row>
+    <row r="88" spans="1:11" s="62" customFormat="1">
+      <c r="A88" s="66"/>
+      <c r="H88" s="66"/>
+      <c r="I88" s="66"/>
+      <c r="J88" s="66"/>
+      <c r="K88" s="66"/>
+    </row>
+    <row r="89" spans="1:11" s="62" customFormat="1">
+      <c r="A89" s="66"/>
+      <c r="H89" s="66"/>
+      <c r="I89" s="66"/>
+      <c r="J89" s="66"/>
+      <c r="K89" s="66"/>
+    </row>
+    <row r="90" spans="1:11" s="62" customFormat="1">
+      <c r="A90" s="66"/>
+      <c r="H90" s="66"/>
+      <c r="I90" s="66"/>
+      <c r="J90" s="66"/>
+      <c r="K90" s="66"/>
+    </row>
+    <row r="91" spans="1:11" s="62" customFormat="1">
+      <c r="A91" s="66"/>
+      <c r="H91" s="66"/>
+      <c r="I91" s="66"/>
+      <c r="J91" s="66"/>
+      <c r="K91" s="66"/>
+    </row>
+    <row r="92" spans="1:11" s="62" customFormat="1">
+      <c r="A92" s="66"/>
+      <c r="H92" s="66"/>
+      <c r="I92" s="66"/>
+      <c r="J92" s="66"/>
+      <c r="K92" s="66"/>
+    </row>
+    <row r="93" spans="1:11" s="62" customFormat="1">
+      <c r="A93" s="66"/>
+      <c r="H93" s="66"/>
+      <c r="I93" s="66"/>
+      <c r="J93" s="66"/>
+      <c r="K93" s="66"/>
+    </row>
+    <row r="94" spans="1:11" s="62" customFormat="1">
+      <c r="A94" s="66"/>
+      <c r="H94" s="66"/>
+      <c r="I94" s="66"/>
+      <c r="J94" s="66"/>
+      <c r="K94" s="66"/>
+    </row>
+    <row r="95" spans="1:11" s="62" customFormat="1">
+      <c r="A95" s="66"/>
+      <c r="H95" s="66"/>
+      <c r="I95" s="66"/>
+      <c r="J95" s="66"/>
+      <c r="K95" s="66"/>
+    </row>
+    <row r="96" spans="1:11" s="62" customFormat="1">
+      <c r="A96" s="66"/>
+      <c r="H96" s="66"/>
+      <c r="I96" s="66"/>
+      <c r="J96" s="66"/>
+      <c r="K96" s="66"/>
+    </row>
+    <row r="97" spans="1:11" s="62" customFormat="1">
+      <c r="A97" s="66"/>
+      <c r="H97" s="66"/>
+      <c r="I97" s="66"/>
+      <c r="J97" s="66"/>
+      <c r="K97" s="66"/>
+    </row>
+    <row r="98" spans="1:11" s="62" customFormat="1">
+      <c r="A98" s="66"/>
+      <c r="H98" s="66"/>
+      <c r="I98" s="66"/>
+      <c r="J98" s="66"/>
+      <c r="K98" s="66"/>
+    </row>
+    <row r="99" spans="1:11" s="62" customFormat="1">
+      <c r="A99" s="66"/>
+      <c r="H99" s="66"/>
+      <c r="I99" s="66"/>
+      <c r="J99" s="66"/>
+      <c r="K99" s="66"/>
+    </row>
+    <row r="100" spans="1:11" s="62" customFormat="1">
+      <c r="A100" s="66"/>
+      <c r="H100" s="66"/>
+      <c r="I100" s="66"/>
+      <c r="J100" s="66"/>
+      <c r="K100" s="66"/>
+    </row>
+    <row r="101" spans="1:11" s="62" customFormat="1">
+      <c r="A101" s="66"/>
+      <c r="H101" s="66"/>
+      <c r="I101" s="66"/>
+      <c r="J101" s="66"/>
+      <c r="K101" s="66"/>
+    </row>
+    <row r="102" spans="1:11" s="62" customFormat="1">
+      <c r="A102" s="2"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
+  <mergeCells count="64">
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K15:K19"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="B35:C39"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C27"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H33:I33"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="K23:K27"/>
-    <mergeCell ref="D23:E27"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G27"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K28:K32"/>
+    <mergeCell ref="D28:E32"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G32"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="F34:G38"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B40:C44"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="D40:E44"/>
+    <mergeCell ref="F40:G44"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B34:C38"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F15:G19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="H35:I35">
+  <conditionalFormatting sqref="H40:I40">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:I34">
+  <conditionalFormatting sqref="H39:I39">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Test case update 2
</commit_message>
<xml_diff>
--- a/Project_Code_Testcase_Template_v2.2.xlsx
+++ b/Project_Code_Testcase_Template_v2.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nam4-1\Quan Tri Du An\QuanTriDuAnCNTT-CNTT-20181\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1D0CE496-6F6F-4E48-A396-5C94805316ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC2CB23F-CF0D-46BB-87EF-C6465B6100E7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$66</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="84">
   <si>
     <t>Online ID</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Resp</t>
   </si>
   <si>
-    <t>23/08/2008</t>
-  </si>
-  <si>
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>2.</t>
   </si>
   <si>
-    <t>1.2.2-2</t>
-  </si>
-  <si>
     <t>Test case Overview</t>
   </si>
   <si>
@@ -284,24 +278,12 @@
     <t>Not OK</t>
   </si>
   <si>
-    <t>TienND</t>
-  </si>
-  <si>
     <t>Test Date</t>
   </si>
   <si>
     <t>Repairer</t>
   </si>
   <si>
-    <t>AnhDV</t>
-  </si>
-  <si>
-    <t>20/08/2008</t>
-  </si>
-  <si>
-    <t>DinhPX</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -311,115 +293,157 @@
     <t>Related Software:</t>
   </si>
   <si>
-    <t>Xem được phim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Mpeg
+    <t>BUG213</t>
+  </si>
+  <si>
+    <t>Tested and result is correct</t>
+  </si>
+  <si>
+    <t>Tested and result is not correct</t>
+  </si>
+  <si>
+    <t>Pending test</t>
+  </si>
+  <si>
+    <t>Project:</t>
+  </si>
+  <si>
+    <t>Result:</t>
+  </si>
+  <si>
+    <t>OK:</t>
+  </si>
+  <si>
+    <t>Not OK:</t>
+  </si>
+  <si>
+    <t>Untested:</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>(SheetNo).(Med Point).(Sub Point)-(Testcase ID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Operation Test</t>
+  </si>
+  <si>
+    <t>Big Point:</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ID Fmt:</t>
+  </si>
+  <si>
+    <t>Hear and Note</t>
+  </si>
+  <si>
+    <t>Test đăng nhập</t>
+  </si>
+  <si>
+    <t>Không nhập tài khoản hoặc mật khẩu</t>
+  </si>
+  <si>
+    <t>chỉ nhập tên tài khoản hoặc mật khẩu, hoặc không nhập cả tài khoản và mật khẩu</t>
+  </si>
+  <si>
+    <t>hiển thị thông báo yêu cầu nhập tài khoản, mật khẩu</t>
+  </si>
+  <si>
+    <t>DungVV</t>
+  </si>
+  <si>
+    <t>14/12/2018</t>
+  </si>
+  <si>
+    <t>Nhập sai mật khẩu</t>
+  </si>
+  <si>
+    <t>nhập mật khẩu sai</t>
+  </si>
+  <si>
+    <t>hiển thị thông báo nhập mật khẩu sai, yêu cầu nhập lại mật khẩu</t>
+  </si>
+  <si>
+    <t>1.1-3</t>
+  </si>
+  <si>
+    <t>nhập đúng tài khoản và mật khẩu</t>
+  </si>
+  <si>
+    <t>nhập tài khoản và mật khẩu đã được tạo</t>
+  </si>
+  <si>
+    <t>đăng nhập thành công</t>
+  </si>
+  <si>
+    <t>Phân biệt chữ hoa chữ thường</t>
+  </si>
+  <si>
+    <t>2.1-1</t>
+  </si>
+  <si>
+    <t>test chức năng tìm kiếm</t>
+  </si>
+  <si>
+    <t>1. Nhập thông tin tìm kiếm bằng chữ thường
+2. thông tin tìm kiếm bao gồm cả chữ hoa
+3. nhấn tìm kiếm</t>
+  </si>
+  <si>
+    <t>Tìm được thông tin yêu cầu</t>
+  </si>
+  <si>
+    <t>15/12/2018</t>
+  </si>
+  <si>
+    <t>2.1-2</t>
+  </si>
+  <si>
+    <t>2.1-3</t>
+  </si>
+  <si>
+    <t>Nhập thừa dấu cách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. nhập thông tin tìm kiếm mà có nhiều khoảng trắng
+2. nhấn tìm kiếm
 </t>
   </si>
   <si>
-    <t>1. Add film mpeg
-2. Mo VLC
-3. Gõ địa chỉ 192.168.0.5</t>
-  </si>
-  <si>
-    <t>File Mpeg có thời lượng 3s</t>
-  </si>
-  <si>
-    <t>BUG213</t>
-  </si>
-  <si>
-    <t>Tested and result is correct</t>
-  </si>
-  <si>
-    <t>Tested and result is not correct</t>
-  </si>
-  <si>
-    <t>Pending test</t>
-  </si>
-  <si>
-    <t>Project:</t>
-  </si>
-  <si>
-    <t>Result:</t>
-  </si>
-  <si>
-    <t>OK:</t>
-  </si>
-  <si>
-    <t>Not OK:</t>
-  </si>
-  <si>
-    <t>Untested:</t>
-  </si>
-  <si>
-    <t>Total:</t>
-  </si>
-  <si>
-    <t>(SheetNo).(Med Point).(Sub Point)-(Testcase ID)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Operation Test</t>
-  </si>
-  <si>
-    <t>Big Point:</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>ID Fmt:</t>
-  </si>
-  <si>
-    <t>Hear and Note</t>
-  </si>
-  <si>
-    <t>Test đăng nhập</t>
-  </si>
-  <si>
-    <t>Không nhập tài khoản hoặc mật khẩu</t>
-  </si>
-  <si>
-    <t>chỉ nhập tên tài khoản hoặc mật khẩu, hoặc không nhập cả tài khoản và mật khẩu</t>
-  </si>
-  <si>
-    <t>hiển thị thông báo yêu cầu nhập tài khoản, mật khẩu</t>
-  </si>
-  <si>
-    <t>DungVV</t>
-  </si>
-  <si>
-    <t>14/12/2018</t>
-  </si>
-  <si>
-    <t>Nhập sai mật khẩu</t>
-  </si>
-  <si>
-    <t>nhập mật khẩu sai</t>
-  </si>
-  <si>
-    <t>hiển thị thông báo nhập mật khẩu sai, yêu cầu nhập lại mật khẩu</t>
-  </si>
-  <si>
-    <t>1.1-3</t>
-  </si>
-  <si>
-    <t>nhập đúng tài khoản và mật khẩu</t>
-  </si>
-  <si>
-    <t>nhập tài khoản và mật khẩu đã được tạo</t>
-  </si>
-  <si>
-    <t>đăng nhập thành công</t>
-  </si>
-  <si>
-    <t>Test chức năng</t>
+    <t>Thông tin nhập vào tìm kiếm không theo trật tự</t>
+  </si>
+  <si>
+    <t>1. Nhập từ khóa tìm kiếm không theo trình tự
+2. Nhấn tìm kiếm</t>
+  </si>
+  <si>
+    <t>HangNT</t>
+  </si>
+  <si>
+    <t>KhiemND</t>
+  </si>
+  <si>
+    <t>2.1-4</t>
+  </si>
+  <si>
+    <t>Thông tin tìm kiếm không có.</t>
+  </si>
+  <si>
+    <t>1. Nhập từ khóa tìm kiếm
+2. Nhấn tìm kiếm</t>
+  </si>
+  <si>
+    <t>Hiển thị thông báo không tìm kiếm được</t>
   </si>
 </sst>
 </file>
@@ -936,7 +960,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1213,6 +1237,30 @@
     <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1220,6 +1268,57 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1229,24 +1328,6 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1256,45 +1337,12 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1304,8 +1352,23 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1313,54 +1376,35 @@
     <xf numFmtId="14" fontId="21" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1828,7 +1872,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1909,13 +1953,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="120"/>
-      <c r="Q6" s="120"/>
-      <c r="R6" s="120"/>
-      <c r="S6" s="120"/>
+      <c r="O6" s="128" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="128"/>
+      <c r="Q6" s="128"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="128"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1925,11 +1969,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="120"/>
-      <c r="P7" s="120"/>
-      <c r="Q7" s="120"/>
-      <c r="R7" s="120"/>
-      <c r="S7" s="120"/>
+      <c r="O7" s="128"/>
+      <c r="P7" s="128"/>
+      <c r="Q7" s="128"/>
+      <c r="R7" s="128"/>
+      <c r="S7" s="128"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -1944,10 +1988,10 @@
       <c r="B9" s="30"/>
       <c r="C9" s="18"/>
       <c r="D9" s="27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1958,7 +2002,7 @@
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
@@ -1968,7 +2012,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="117" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
@@ -1982,34 +2026,34 @@
       <c r="B11" s="30"/>
       <c r="C11" s="18"/>
       <c r="D11" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="121">
+        <v>9</v>
+      </c>
+      <c r="E11" s="129">
         <f ca="1">TODAY()</f>
-        <v>43448</v>
-      </c>
-      <c r="F11" s="121"/>
-      <c r="G11" s="121"/>
+        <v>43449</v>
+      </c>
+      <c r="F11" s="129"/>
+      <c r="G11" s="129"/>
       <c r="H11" s="76"/>
       <c r="L11" s="33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V11" s="33"/>
       <c r="X11" s="19"/>
@@ -2017,7 +2061,7 @@
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
       <c r="L12" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -2095,7 +2139,7 @@
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="75"/>
@@ -2226,7 +2270,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="L19" s="36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
@@ -2278,7 +2322,7 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E22" s="75"/>
       <c r="F22" s="75"/>
@@ -2305,7 +2349,7 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="L24" s="117" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M24" s="107"/>
       <c r="N24" s="107"/>
@@ -2440,7 +2484,7 @@
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
       <c r="C31" s="39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2476,7 +2520,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2546,7 +2590,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2582,7 +2626,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2849,8 +2893,8 @@
   </sheetPr>
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2864,7 +2908,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="62" customFormat="1">
       <c r="A1" s="81" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B1" s="82" t="str">
         <f>Overview!E9</f>
@@ -2875,26 +2919,26 @@
       <c r="E1" s="83"/>
       <c r="F1" s="83"/>
       <c r="G1" s="84" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="I1" s="104">
         <f>COUNTIF(H1:H791,"OK")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J1" s="86" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K1" s="87"/>
     </row>
     <row r="2" spans="1:11" s="62" customFormat="1">
       <c r="A2" s="119" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C2" s="89"/>
       <c r="D2" s="89"/>
@@ -2902,23 +2946,23 @@
       <c r="F2" s="90"/>
       <c r="G2" s="91"/>
       <c r="H2" s="92" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I2" s="105">
         <f>COUNTIF(H2:H792,"Not OK")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2" s="93" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="K2" s="94"/>
     </row>
     <row r="3" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
       <c r="A3" s="88" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C3" s="89"/>
       <c r="D3" s="89"/>
@@ -2926,14 +2970,14 @@
       <c r="F3" s="90"/>
       <c r="G3" s="91"/>
       <c r="H3" s="92" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I3" s="106">
         <f>COUNTIF(H2:H792,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="93" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="K3" s="94"/>
     </row>
@@ -2945,12 +2989,12 @@
       <c r="E4" s="90"/>
       <c r="F4" s="90"/>
       <c r="G4" s="96" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H4" s="89"/>
       <c r="I4" s="105">
         <f>COUNTIF(H3:H793,"Result")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J4" s="93"/>
       <c r="K4" s="94"/>
@@ -2983,435 +3027,435 @@
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
       <c r="A7" s="103" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="147" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="147"/>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="147"/>
-      <c r="H7" s="147"/>
-      <c r="I7" s="147"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="147"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="155" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="155"/>
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="155"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="155"/>
+      <c r="J7" s="155"/>
+      <c r="K7" s="155"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="148"/>
+      <c r="D8" s="147" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="148"/>
+      <c r="F8" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="122" t="s">
+      <c r="G8" s="148"/>
+      <c r="H8" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="122" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="123"/>
-      <c r="F8" s="122" t="s">
+      <c r="I8" s="156"/>
+      <c r="J8" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="123"/>
-      <c r="H8" s="148" t="s">
+      <c r="K8" s="49" t="s">
         <v>25</v>
-      </c>
-      <c r="I8" s="148"/>
-      <c r="J8" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="49" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="125" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="126"/>
-      <c r="D9" s="134" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="135"/>
-      <c r="F9" s="134" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="135"/>
-      <c r="H9" s="140" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="141"/>
+      <c r="B9" s="130" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="131"/>
+      <c r="D9" s="136" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="137"/>
+      <c r="F9" s="136" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="137"/>
+      <c r="H9" s="153" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="154"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="144"/>
+      <c r="K9" s="142"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="132"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="47" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="127"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="47" t="s">
-        <v>30</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="145"/>
+        <v>31</v>
+      </c>
+      <c r="K10" s="143"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="127"/>
-      <c r="C11" s="128"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="137"/>
+        <v>3</v>
+      </c>
+      <c r="B11" s="132"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="138"/>
+      <c r="E11" s="139"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="139"/>
       <c r="H11" s="52" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I11" s="52"/>
       <c r="J11" s="50"/>
-      <c r="K11" s="145"/>
+      <c r="K11" s="143"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="127"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="137"/>
-      <c r="F12" s="136"/>
-      <c r="G12" s="137"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="138"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="139"/>
       <c r="H12" s="47" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J12" s="47"/>
-      <c r="K12" s="145"/>
+      <c r="K12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="53">
         <v>981</v>
       </c>
-      <c r="B13" s="129"/>
-      <c r="C13" s="130"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="139"/>
+      <c r="B13" s="134"/>
+      <c r="C13" s="135"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="141"/>
+      <c r="F13" s="140"/>
+      <c r="G13" s="141"/>
       <c r="H13" s="55" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I13" s="55"/>
       <c r="J13" s="56"/>
-      <c r="K13" s="146"/>
+      <c r="K13" s="144"/>
     </row>
     <row r="14" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A14" s="153" t="s">
+      <c r="A14" s="123" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="167" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="168"/>
+      <c r="D14" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="168"/>
+      <c r="F14" s="167" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="154" t="s">
+      <c r="G14" s="168"/>
+      <c r="H14" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="155"/>
-      <c r="F14" s="154" t="s">
+      <c r="I14" s="166"/>
+      <c r="J14" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="155"/>
-      <c r="H14" s="156" t="s">
+      <c r="K14" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="156"/>
-      <c r="J14" s="157" t="s">
+    </row>
+    <row r="15" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A15" s="122">
+        <v>2</v>
+      </c>
+      <c r="B15" s="158" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="159"/>
+      <c r="D15" s="136" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="137"/>
+      <c r="F15" s="136" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="137"/>
+      <c r="H15" s="164" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="165"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="142"/>
+    </row>
+    <row r="16" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A16" s="123" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="158" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A15" s="150">
-        <v>2</v>
-      </c>
-      <c r="B15" s="159" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="160"/>
-      <c r="D15" s="134" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="135"/>
-      <c r="F15" s="134" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="135"/>
-      <c r="H15" s="151" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="152"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="144"/>
-    </row>
-    <row r="16" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="B16" s="160"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="138"/>
+      <c r="G16" s="139"/>
+      <c r="H16" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="161"/>
-      <c r="C16" s="162"/>
-      <c r="D16" s="136"/>
-      <c r="E16" s="137"/>
-      <c r="F16" s="136"/>
-      <c r="G16" s="137"/>
-      <c r="H16" s="165" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="165" t="s">
+      <c r="I16" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="J16" s="166" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="145"/>
+      <c r="J16" s="127" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="143"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A17" s="150" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="161"/>
-      <c r="C17" s="162"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="137"/>
+      <c r="A17" s="122" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="160"/>
+      <c r="C17" s="161"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="139"/>
       <c r="H17" s="55" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I17" s="55"/>
       <c r="J17" s="56"/>
-      <c r="K17" s="145"/>
+      <c r="K17" s="143"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="153" t="s">
+      <c r="A18" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="161"/>
-      <c r="C18" s="162"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="137"/>
-      <c r="F18" s="136"/>
-      <c r="G18" s="137"/>
-      <c r="H18" s="165" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="165" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="166"/>
-      <c r="K18" s="145"/>
+      <c r="B18" s="160"/>
+      <c r="C18" s="161"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="126" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="126" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="127"/>
+      <c r="K18" s="143"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A19" s="150">
+      <c r="A19" s="122">
         <v>933</v>
       </c>
-      <c r="B19" s="163"/>
-      <c r="C19" s="164"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="139"/>
-      <c r="F19" s="138"/>
-      <c r="G19" s="139"/>
+      <c r="B19" s="162"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="141"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="141"/>
       <c r="H19" s="55" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I19" s="55"/>
       <c r="J19" s="56"/>
-      <c r="K19" s="146"/>
+      <c r="K19" s="144"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A20" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="151" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="152"/>
+      <c r="D20" s="151" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="152"/>
+      <c r="F20" s="151" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="132" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="133"/>
-      <c r="D20" s="132" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="133"/>
-      <c r="F20" s="132" t="s">
+      <c r="G20" s="152"/>
+      <c r="H20" s="150" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="150"/>
+      <c r="J20" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="133"/>
-      <c r="H20" s="131" t="s">
+      <c r="K20" s="58" t="s">
         <v>25</v>
-      </c>
-      <c r="I20" s="131"/>
-      <c r="J20" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="58" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="50">
         <v>3</v>
       </c>
-      <c r="B21" s="125" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="126"/>
-      <c r="D21" s="134" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="135"/>
-      <c r="F21" s="134" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="135"/>
-      <c r="H21" s="142" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="143"/>
+      <c r="B21" s="130" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="131"/>
+      <c r="D21" s="136" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="137"/>
+      <c r="F21" s="136" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="137"/>
+      <c r="H21" s="145" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="146"/>
       <c r="J21" s="54"/>
-      <c r="K21" s="144"/>
+      <c r="K21" s="142"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="132"/>
+      <c r="C22" s="133"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="59" t="s">
         <v>28</v>
-      </c>
-      <c r="B22" s="127"/>
-      <c r="C22" s="128"/>
-      <c r="D22" s="136"/>
-      <c r="E22" s="137"/>
-      <c r="F22" s="136"/>
-      <c r="G22" s="137"/>
-      <c r="H22" s="59" t="s">
-        <v>30</v>
       </c>
       <c r="I22" s="59" t="s">
         <v>1</v>
       </c>
       <c r="J22" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="145"/>
+        <v>31</v>
+      </c>
+      <c r="K22" s="143"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="127"/>
-      <c r="C23" s="128"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="137"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="137"/>
+        <v>62</v>
+      </c>
+      <c r="B23" s="132"/>
+      <c r="C23" s="133"/>
+      <c r="D23" s="138"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="138"/>
+      <c r="G23" s="139"/>
       <c r="H23" s="52" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I23" s="52"/>
       <c r="J23" s="50"/>
-      <c r="K23" s="145"/>
+      <c r="K23" s="143"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="127"/>
-      <c r="C24" s="128"/>
-      <c r="D24" s="136"/>
-      <c r="E24" s="137"/>
-      <c r="F24" s="136"/>
-      <c r="G24" s="137"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="139"/>
       <c r="H24" s="59" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I24" s="59" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J24" s="59"/>
-      <c r="K24" s="145"/>
+      <c r="K24" s="143"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53">
         <v>921</v>
       </c>
-      <c r="B25" s="129"/>
-      <c r="C25" s="130"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="139"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="139"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="140"/>
+      <c r="E25" s="141"/>
+      <c r="F25" s="140"/>
+      <c r="G25" s="141"/>
       <c r="H25" s="52" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I25" s="52"/>
       <c r="J25" s="50"/>
-      <c r="K25" s="145"/>
+      <c r="K25" s="143"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="149" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="149"/>
-      <c r="D26" s="147"/>
-      <c r="E26" s="147"/>
-      <c r="F26" s="147"/>
-      <c r="G26" s="147"/>
-      <c r="H26" s="147"/>
-      <c r="I26" s="147"/>
-      <c r="J26" s="147"/>
-      <c r="K26" s="147"/>
+        <v>6</v>
+      </c>
+      <c r="B26" s="157" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="157"/>
+      <c r="D26" s="155"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="155"/>
+      <c r="H26" s="155"/>
+      <c r="I26" s="155"/>
+      <c r="J26" s="155"/>
+      <c r="K26" s="155"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="151" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="152"/>
+      <c r="D27" s="151" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="152"/>
+      <c r="F27" s="151" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="132" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="133"/>
-      <c r="D27" s="132" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="133"/>
-      <c r="F27" s="132" t="s">
+      <c r="G27" s="152"/>
+      <c r="H27" s="150" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="150"/>
+      <c r="J27" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="133"/>
-      <c r="H27" s="131" t="s">
+      <c r="K27" s="59" t="s">
         <v>25</v>
-      </c>
-      <c r="I27" s="131"/>
-      <c r="J27" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="59" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
@@ -3419,408 +3463,476 @@
         <f>A21+1</f>
         <v>4</v>
       </c>
-      <c r="B28" s="125" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="126"/>
-      <c r="D28" s="134" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="135"/>
-      <c r="F28" s="134" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" s="135"/>
-      <c r="H28" s="140" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="141"/>
+      <c r="B28" s="130" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="131"/>
+      <c r="D28" s="136" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="137"/>
+      <c r="F28" s="136" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="137"/>
+      <c r="H28" s="153" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="154"/>
       <c r="J28" s="50"/>
-      <c r="K28" s="144"/>
+      <c r="K28" s="142"/>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="132"/>
+      <c r="C29" s="133"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="138"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="59" t="s">
         <v>28</v>
-      </c>
-      <c r="B29" s="127"/>
-      <c r="C29" s="128"/>
-      <c r="D29" s="136"/>
-      <c r="E29" s="137"/>
-      <c r="F29" s="136"/>
-      <c r="G29" s="137"/>
-      <c r="H29" s="59" t="s">
-        <v>30</v>
       </c>
       <c r="I29" s="59" t="s">
         <v>1</v>
       </c>
       <c r="J29" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="145"/>
+        <v>31</v>
+      </c>
+      <c r="K29" s="143"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="127"/>
-      <c r="C30" s="128"/>
-      <c r="D30" s="136"/>
-      <c r="E30" s="137"/>
-      <c r="F30" s="136"/>
-      <c r="G30" s="137"/>
+        <v>67</v>
+      </c>
+      <c r="B30" s="132"/>
+      <c r="C30" s="133"/>
+      <c r="D30" s="138"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="138"/>
+      <c r="G30" s="139"/>
       <c r="H30" s="52" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I30" s="52"/>
       <c r="J30" s="50"/>
-      <c r="K30" s="145"/>
+      <c r="K30" s="143"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="127"/>
-      <c r="C31" s="128"/>
-      <c r="D31" s="136"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="136"/>
-      <c r="G31" s="137"/>
+      <c r="B31" s="132"/>
+      <c r="C31" s="133"/>
+      <c r="D31" s="138"/>
+      <c r="E31" s="139"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="139"/>
       <c r="H31" s="59" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I31" s="59"/>
       <c r="J31" s="59"/>
-      <c r="K31" s="145"/>
+      <c r="K31" s="143"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="53">
         <v>922</v>
       </c>
-      <c r="B32" s="129"/>
-      <c r="C32" s="130"/>
-      <c r="D32" s="138"/>
-      <c r="E32" s="139"/>
-      <c r="F32" s="138"/>
-      <c r="G32" s="139"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="135"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="141"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="141"/>
       <c r="H32" s="52" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="I32" s="52"/>
       <c r="J32" s="50"/>
-      <c r="K32" s="146"/>
+      <c r="K32" s="144"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="148"/>
+      <c r="D33" s="147" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="148"/>
+      <c r="F33" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="122" t="s">
+      <c r="G33" s="148"/>
+      <c r="H33" s="149" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="123"/>
-      <c r="D33" s="122" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="123"/>
-      <c r="F33" s="122" t="s">
+      <c r="I33" s="149"/>
+      <c r="J33" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="123"/>
-      <c r="H33" s="124" t="s">
+      <c r="K33" s="60" t="s">
         <v>25</v>
-      </c>
-      <c r="I33" s="124"/>
-      <c r="J33" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" s="60" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="50">
-        <v>4</v>
-      </c>
-      <c r="B34" s="125" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="126"/>
-      <c r="D34" s="134" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="135"/>
-      <c r="F34" s="134" t="s">
-        <v>41</v>
-      </c>
-      <c r="G34" s="135"/>
-      <c r="H34" s="142" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="143"/>
-      <c r="J34" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="K34" s="144"/>
+        <v>5</v>
+      </c>
+      <c r="B34" s="130" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="131"/>
+      <c r="D34" s="136" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="137"/>
+      <c r="F34" s="136" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" s="137"/>
+      <c r="H34" s="145" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="146"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="142"/>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="132"/>
+      <c r="C35" s="133"/>
+      <c r="D35" s="138"/>
+      <c r="E35" s="139"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="47" t="s">
         <v>28</v>
-      </c>
-      <c r="B35" s="127"/>
-      <c r="C35" s="128"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="137"/>
-      <c r="F35" s="136"/>
-      <c r="G35" s="137"/>
-      <c r="H35" s="47" t="s">
-        <v>30</v>
       </c>
       <c r="I35" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J35" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35" s="145"/>
+        <v>31</v>
+      </c>
+      <c r="K35" s="143"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="127"/>
-      <c r="C36" s="128"/>
-      <c r="D36" s="136"/>
-      <c r="E36" s="137"/>
-      <c r="F36" s="136"/>
-      <c r="G36" s="137"/>
+        <v>72</v>
+      </c>
+      <c r="B36" s="132"/>
+      <c r="C36" s="133"/>
+      <c r="D36" s="138"/>
+      <c r="E36" s="139"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="139"/>
       <c r="H36" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="I36" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="K36" s="145"/>
+        <v>57</v>
+      </c>
+      <c r="I36" s="52"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="143"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="127"/>
-      <c r="C37" s="128"/>
-      <c r="D37" s="136"/>
-      <c r="E37" s="137"/>
-      <c r="F37" s="136"/>
-      <c r="G37" s="137"/>
+      <c r="B37" s="132"/>
+      <c r="C37" s="133"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="139"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="139"/>
       <c r="H37" s="47" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I37" s="47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J37" s="47"/>
-      <c r="K37" s="145"/>
+      <c r="K37" s="143"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="53">
-        <v>823</v>
-      </c>
-      <c r="B38" s="129"/>
-      <c r="C38" s="130"/>
-      <c r="D38" s="138"/>
-      <c r="E38" s="139"/>
-      <c r="F38" s="138"/>
-      <c r="G38" s="139"/>
+        <v>888</v>
+      </c>
+      <c r="B38" s="134"/>
+      <c r="C38" s="135"/>
+      <c r="D38" s="140"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="141"/>
       <c r="H38" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="I38" s="52" t="s">
-        <v>2</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I38" s="52"/>
       <c r="J38" s="50"/>
-      <c r="K38" s="146"/>
+      <c r="K38" s="144"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="148"/>
+      <c r="D39" s="147" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="148"/>
+      <c r="F39" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="122" t="s">
+      <c r="G39" s="148"/>
+      <c r="H39" s="149" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="123"/>
-      <c r="D39" s="122" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="123"/>
-      <c r="F39" s="122" t="s">
+      <c r="I39" s="149"/>
+      <c r="J39" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="123"/>
-      <c r="H39" s="124" t="s">
+      <c r="K39" s="60" t="s">
         <v>25</v>
-      </c>
-      <c r="I39" s="124"/>
-      <c r="J39" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="K39" s="60" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A40" s="50">
-        <v>5</v>
-      </c>
-      <c r="B40" s="125" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="126"/>
-      <c r="D40" s="134" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40" s="135"/>
-      <c r="F40" s="134" t="s">
-        <v>41</v>
-      </c>
-      <c r="G40" s="135"/>
-      <c r="H40" s="142" t="s">
-        <v>31</v>
-      </c>
-      <c r="I40" s="143"/>
+        <v>6</v>
+      </c>
+      <c r="B40" s="130" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="131"/>
+      <c r="D40" s="136" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="137"/>
+      <c r="F40" s="136" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="137"/>
+      <c r="H40" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="146"/>
       <c r="J40" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="K40" s="144"/>
+        <v>35</v>
+      </c>
+      <c r="K40" s="142"/>
     </row>
     <row r="41" spans="1:11" ht="10.5" customHeight="1">
       <c r="A41" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="132"/>
+      <c r="C41" s="133"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="139"/>
+      <c r="F41" s="138"/>
+      <c r="G41" s="139"/>
+      <c r="H41" s="47" t="s">
         <v>28</v>
-      </c>
-      <c r="B41" s="127"/>
-      <c r="C41" s="128"/>
-      <c r="D41" s="136"/>
-      <c r="E41" s="137"/>
-      <c r="F41" s="136"/>
-      <c r="G41" s="137"/>
-      <c r="H41" s="47" t="s">
-        <v>30</v>
       </c>
       <c r="I41" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J41" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="K41" s="145"/>
+        <v>31</v>
+      </c>
+      <c r="K41" s="143"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="127"/>
-      <c r="C42" s="128"/>
-      <c r="D42" s="136"/>
-      <c r="E42" s="137"/>
-      <c r="F42" s="136"/>
-      <c r="G42" s="137"/>
+        <v>73</v>
+      </c>
+      <c r="B42" s="132"/>
+      <c r="C42" s="133"/>
+      <c r="D42" s="138"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="138"/>
+      <c r="G42" s="139"/>
       <c r="H42" s="52" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I42" s="52" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="J42" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="K42" s="145"/>
+        <v>78</v>
+      </c>
+      <c r="K42" s="143"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="127"/>
-      <c r="C43" s="128"/>
-      <c r="D43" s="136"/>
-      <c r="E43" s="137"/>
-      <c r="F43" s="136"/>
-      <c r="G43" s="137"/>
+      <c r="B43" s="132"/>
+      <c r="C43" s="133"/>
+      <c r="D43" s="138"/>
+      <c r="E43" s="139"/>
+      <c r="F43" s="138"/>
+      <c r="G43" s="139"/>
       <c r="H43" s="47" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I43" s="47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J43" s="47"/>
-      <c r="K43" s="145"/>
+      <c r="K43" s="143"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="53">
         <v>823</v>
       </c>
-      <c r="B44" s="129"/>
-      <c r="C44" s="130"/>
-      <c r="D44" s="138"/>
-      <c r="E44" s="139"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="139"/>
+      <c r="B44" s="134"/>
+      <c r="C44" s="135"/>
+      <c r="D44" s="140"/>
+      <c r="E44" s="141"/>
+      <c r="F44" s="140"/>
+      <c r="G44" s="141"/>
       <c r="H44" s="52" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="I44" s="52" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="J44" s="50"/>
-      <c r="K44" s="146"/>
+      <c r="K44" s="144"/>
     </row>
     <row r="45" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A45" s="66"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="66"/>
-      <c r="I45" s="66"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="66"/>
-    </row>
-    <row r="46" spans="1:11" s="62" customFormat="1">
-      <c r="A46" s="66"/>
-      <c r="H46" s="66"/>
-      <c r="I46" s="66"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="66"/>
-    </row>
-    <row r="47" spans="1:11" s="62" customFormat="1">
-      <c r="A47" s="66"/>
-      <c r="H47" s="66"/>
-      <c r="I47" s="66"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="66"/>
-    </row>
-    <row r="48" spans="1:11" s="62" customFormat="1">
-      <c r="A48" s="66"/>
-      <c r="H48" s="66"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="66"/>
-      <c r="K48" s="66"/>
-    </row>
-    <row r="49" spans="1:11" s="62" customFormat="1">
-      <c r="A49" s="66"/>
-      <c r="H49" s="66"/>
-      <c r="I49" s="66"/>
-      <c r="J49" s="66"/>
-      <c r="K49" s="66"/>
-    </row>
-    <row r="50" spans="1:11" s="62" customFormat="1">
-      <c r="A50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
+      <c r="A45" s="121" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="148"/>
+      <c r="D45" s="147" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="148"/>
+      <c r="F45" s="147" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="148"/>
+      <c r="H45" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="149"/>
+      <c r="J45" s="121" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="120" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A46" s="50">
+        <v>7</v>
+      </c>
+      <c r="B46" s="130" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="131"/>
+      <c r="D46" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="137"/>
+      <c r="F46" s="136" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="137"/>
+      <c r="H46" s="145" t="s">
+        <v>32</v>
+      </c>
+      <c r="I46" s="146"/>
+      <c r="J46" s="54"/>
+      <c r="K46" s="142"/>
+    </row>
+    <row r="47" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A47" s="121" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="132"/>
+      <c r="C47" s="133"/>
+      <c r="D47" s="138"/>
+      <c r="E47" s="139"/>
+      <c r="F47" s="138"/>
+      <c r="G47" s="139"/>
+      <c r="H47" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="121" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" s="121" t="s">
+        <v>31</v>
+      </c>
+      <c r="K47" s="143"/>
+    </row>
+    <row r="48" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A48" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="132"/>
+      <c r="C48" s="133"/>
+      <c r="D48" s="138"/>
+      <c r="E48" s="139"/>
+      <c r="F48" s="138"/>
+      <c r="G48" s="139"/>
+      <c r="H48" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="I48" s="52"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="143"/>
+    </row>
+    <row r="49" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A49" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="132"/>
+      <c r="C49" s="133"/>
+      <c r="D49" s="138"/>
+      <c r="E49" s="139"/>
+      <c r="F49" s="138"/>
+      <c r="G49" s="139"/>
+      <c r="H49" s="121" t="s">
+        <v>30</v>
+      </c>
+      <c r="I49" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="J49" s="121"/>
+      <c r="K49" s="143"/>
+    </row>
+    <row r="50" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A50" s="53">
+        <v>917</v>
+      </c>
+      <c r="B50" s="134"/>
+      <c r="C50" s="135"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="141"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="141"/>
+      <c r="H50" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="I50" s="52"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="144"/>
     </row>
     <row r="51" spans="1:11" s="62" customFormat="1">
       <c r="A51" s="66"/>
@@ -4193,20 +4305,13 @@
       <c r="K102" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="D15:E19"/>
+  <mergeCells count="73">
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="K15:K19"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="H8:I8"/>
@@ -4228,44 +4333,70 @@
     <mergeCell ref="K34:K38"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B40:C44"/>
-    <mergeCell ref="D34:E38"/>
-    <mergeCell ref="D40:E44"/>
-    <mergeCell ref="F40:G44"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="D9:E13"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:C32"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D21:E25"/>
     <mergeCell ref="B21:C25"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="B34:C38"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F15:G19"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B40:C44"/>
+    <mergeCell ref="D40:E44"/>
+    <mergeCell ref="F40:G44"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:E50"/>
+    <mergeCell ref="F46:G50"/>
+    <mergeCell ref="K46:K50"/>
+    <mergeCell ref="H46:I46"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H40:I40">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39:I39">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46:I46">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39:I39">
+  <conditionalFormatting sqref="H45:I45">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
@@ -4276,6 +4407,9 @@
     <oddHeader>&amp;LTest Case Table&amp;CBig Point: &amp;A</oddHeader>
     <oddFooter>&amp;LAI&amp;&amp;T-ART&amp;CLiveSpark Project&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="44" max="10" man="1"/>
+  </rowBreaks>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>